<commit_message>
Benchmark: tweak plots for Arduino Uno
</commit_message>
<xml_diff>
--- a/Arduino/Audio Processing Benchmarking/FIR Speed Results.xlsx
+++ b/Arduino/Audio Processing Benchmarking/FIR Speed Results.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="89">
   <si>
     <t>Float</t>
   </si>
@@ -379,11 +379,11 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1007,11 +1007,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="211809792"/>
-        <c:axId val="211811712"/>
+        <c:axId val="45434368"/>
+        <c:axId val="45441024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="211809792"/>
+        <c:axId val="45434368"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -1036,20 +1036,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="211811712"/>
+        <c:crossAx val="45441024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="211811712"/>
+        <c:axId val="45441024"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1075,14 +1074,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="211809792"/>
+        <c:crossAx val="45434368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
@@ -1141,6 +1139,47 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600"/>
+              <a:t>FIR Performance,</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600"/>
+              <a:t>Naïve C</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>(Smaller</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t> is Better)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1412,21 +1451,40 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="215228416"/>
-        <c:axId val="215231104"/>
+        <c:axId val="46501248"/>
+        <c:axId val="46503424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="215228416"/>
+        <c:axId val="46501248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>FIR Length (samples)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="215231104"/>
+        <c:crossAx val="46503424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1434,25 +1492,53 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="215231104"/>
+        <c:axId val="46503424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Duration (microseconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="215228416"/>
+        <c:crossAx val="46501248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.85346158319805399"/>
+          <c:y val="0.40029335261880306"/>
+          <c:w val="0.13112415861312135"/>
+          <c:h val="0.2337048183371167"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1488,12 +1574,34 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1600"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>FIR Filter Scaling (Python, PC)</a:t>
+              <a:rPr lang="en-US" sz="1600"/>
+              <a:t>FIR Performance,</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600"/>
+              <a:t>Naïve C</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>(Smaller</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t> is Better)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1503,108 +1611,262 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
-          <c:xVal>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Arduino Uno'!$C$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>float</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
             <c:numRef>
-              <c:f>Python!$B$9:$B$21</c:f>
+              <c:f>'Arduino Uno'!$B$13:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4096</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>8192</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>16384</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Python!$K$9:$K$21</c:f>
+              <c:f>'Arduino Uno'!$C$13:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>1.4246666666666667</c:v>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>311</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6993125</c:v>
+                  <c:v>622</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.34403125000000001</c:v>
+                  <c:v>1270</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.17789843750000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.13063671874999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.8507812500000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4.2874023437499999E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.52666015625E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.671240234375E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.3727213541666667E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2.42724609375E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.4598795572916665E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.2399495442708334E-2</c:v>
+                  <c:v>2522</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Arduino Uno'!$D$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>int16</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Arduino Uno'!$B$13:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Arduino Uno'!$D$13:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>308</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Arduino Uno'!$E$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>int32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Arduino Uno'!$B$13:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Arduino Uno'!$E$13:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>254</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>503</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
@@ -1615,13 +1877,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="213681280"/>
-        <c:axId val="213683200"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="213681280"/>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="83393536"/>
+        <c:axId val="151900928"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="83393536"/>
         <c:scaling>
-          <c:logBase val="2"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1637,7 +1900,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>FIR Filter Length</a:t>
+                  <a:t>FIR Length (samples)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1648,14 +1911,16 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="low"/>
-        <c:crossAx val="213683200"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="151900928"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-        <c:majorUnit val="4"/>
-      </c:valAx>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="213683200"/>
+        <c:axId val="151900928"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1674,7 +1939,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Time per FIR Tap (usec)</a:t>
+                  <a:t>Duration (microseconds)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1686,14 +1951,23 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213681280"/>
+        <c:crossAx val="83393536"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.85346158319805399"/>
+          <c:y val="0.40029335261880306"/>
+          <c:w val="0.13112415861312135"/>
+          <c:h val="0.2337048183371167"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1729,16 +2003,900 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600"/>
+              <a:t>FIR Filters per Second,</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600"/>
+              <a:t>Naïve C</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>(Bigger </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t>is Better)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Arduino Uno'!$C$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>float</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Arduino Uno'!$B$13:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Arduino Uno'!$G$13:$G$16</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3215.4340836012861</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1607.7170418006431</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>787.40157480314963</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>396.51070578905632</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Arduino Uno'!$H$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>int16</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Arduino Uno'!$B$13:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Arduino Uno'!$H$13:$H$16</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>24390.243902439026</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12658.227848101265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6451.6129032258068</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3246.7532467532469</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Arduino Uno'!$I$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>int32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Arduino Uno'!$B$13:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Arduino Uno'!$I$13:$I$16</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7751.937984496124</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3937.0078740157483</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1988.0715705765408</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>998.00399201596804</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="43686528"/>
+        <c:axId val="70632192"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="43686528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>FIR Length (samples)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="70632192"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="70632192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="48000"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>FIR Filters per Second</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="43686528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="8000"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.85346158319805399"/>
+          <c:y val="0.40029335261880306"/>
+          <c:w val="0.13112415861312135"/>
+          <c:h val="0.2337048183371167"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600"/>
+              <a:t>FIR Performance,</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600"/>
+              <a:t>Naïve C</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>(Bigger </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t>is Better)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Arduino Uno'!$C$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>float</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Arduino Uno'!$B$13:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Arduino Uno'!$G$13:$G$16</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3215.4340836012861</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1607.7170418006431</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>787.40157480314963</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>396.51070578905632</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Arduino Uno'!$H$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>int16</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.7071290944123313E-3"/>
+                  <c:y val="-4.7388252598043142E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Arduino Uno'!$B$13:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Arduino Uno'!$H$13:$H$16</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>24390.243902439026</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12658.227848101265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6451.6129032258068</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3246.7532467532469</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Arduino Uno'!$I$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>int32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Arduino Uno'!$B$13:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Arduino Uno'!$I$13:$I$16</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7751.937984496124</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3937.0078740157483</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1988.0715705765408</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>998.00399201596804</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="83543936"/>
+        <c:axId val="89531136"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="83543936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>FIR Length (samples)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="89531136"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="89531136"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>FIR Filters per Second</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="83543936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.85346158319805399"/>
+          <c:y val="0.40029335261880306"/>
+          <c:w val="0.13112415861312135"/>
+          <c:h val="0.2337048183371167"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
               <a:defRPr/>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>FIR Filter Time (Python, PC)</a:t>
+              <a:t>FIR Filter Scaling (Python, PC)</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1800,48 +2958,48 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Python!$D$9:$D$21</c:f>
+              <c:f>Python!$K$9:$K$21</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>5.698666666666667</c:v>
+                  <c:v>1.4246666666666667</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.5945</c:v>
+                  <c:v>0.6993125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.5045000000000002</c:v>
+                  <c:v>0.34403125000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.6927500000000002</c:v>
+                  <c:v>0.17789843750000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.3607499999999995</c:v>
+                  <c:v>0.13063671874999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.7690000000000001</c:v>
+                  <c:v>6.8507812500000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.97575</c:v>
+                  <c:v>4.2874023437499999E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18.0565</c:v>
+                  <c:v>3.52666015625E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>27.3535</c:v>
+                  <c:v>2.671240234375E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>48.593333333333334</c:v>
+                  <c:v>2.3727213541666667E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>99.42</c:v>
+                  <c:v>2.42724609375E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>201.51333333333332</c:v>
+                  <c:v>2.4598795572916665E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>366.99333333333334</c:v>
+                  <c:v>2.2399495442708334E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1856,11 +3014,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="213699968"/>
-        <c:axId val="213329408"/>
+        <c:axId val="46627840"/>
+        <c:axId val="46630016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="213699968"/>
+        <c:axId val="46627840"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -1883,20 +3041,256 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:crossAx val="46630016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="4"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="46630016"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time per FIR Tap (usec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213329408"/>
+        <c:crossAx val="46627840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>FIR Filter Time (Python, PC)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Python!$B$9:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16384</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Python!$D$9:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>5.698666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5945</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.5045000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.6927500000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.3607499999999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.7690000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.97575</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18.0565</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27.3535</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>48.593333333333334</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>99.42</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>201.51333333333332</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>366.99333333333334</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="46650880"/>
+        <c:axId val="46652800"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="46650880"/>
+        <c:scaling>
+          <c:logBase val="2"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>FIR Filter Length</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="46652800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="213329408"/>
+        <c:axId val="46652800"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1920,21 +3314,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213699968"/>
+        <c:crossAx val="46650880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2216,11 +3608,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="213105280"/>
-        <c:axId val="213107072"/>
+        <c:axId val="46008192"/>
+        <c:axId val="46009728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="213105280"/>
+        <c:axId val="46008192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2229,7 +3621,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213107072"/>
+        <c:crossAx val="46009728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2237,7 +3629,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="213107072"/>
+        <c:axId val="46009728"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2261,21 +3653,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213105280"/>
+        <c:crossAx val="46008192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2339,7 +3729,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2560,11 +3949,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="213993728"/>
-        <c:axId val="214007808"/>
+        <c:axId val="46050304"/>
+        <c:axId val="46052096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="213993728"/>
+        <c:axId val="46050304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2573,7 +3962,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="214007808"/>
+        <c:crossAx val="46052096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2581,7 +3970,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="214007808"/>
+        <c:axId val="46052096"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2605,21 +3994,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213993728"/>
+        <c:crossAx val="46050304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2686,7 +4073,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2904,11 +4290,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="213961728"/>
-        <c:axId val="214926080"/>
+        <c:axId val="46086784"/>
+        <c:axId val="46092672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="213961728"/>
+        <c:axId val="46086784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2917,7 +4303,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="214926080"/>
+        <c:crossAx val="46092672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2925,7 +4311,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="214926080"/>
+        <c:axId val="46092672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2962,7 +4348,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213961728"/>
+        <c:crossAx val="46086784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10000"/>
@@ -2970,7 +4356,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3037,7 +4422,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3264,11 +4648,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="213148416"/>
-        <c:axId val="213149952"/>
+        <c:axId val="46123648"/>
+        <c:axId val="45814144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="213148416"/>
+        <c:axId val="46123648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3277,7 +4661,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="213149952"/>
+        <c:crossAx val="45814144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3285,7 +4669,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="213149952"/>
+        <c:axId val="45814144"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3328,7 +4712,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213148416"/>
+        <c:crossAx val="46123648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3411,7 +4795,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3629,11 +5012,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="188019072"/>
-        <c:axId val="188020608"/>
+        <c:axId val="45836544"/>
+        <c:axId val="45838336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="188019072"/>
+        <c:axId val="45836544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3642,7 +5025,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="188020608"/>
+        <c:crossAx val="45838336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3650,7 +5033,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="188020608"/>
+        <c:axId val="45838336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3687,7 +5070,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="188019072"/>
+        <c:crossAx val="45836544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3995,11 +5378,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="102500224"/>
-        <c:axId val="102539648"/>
+        <c:axId val="45877120"/>
+        <c:axId val="45878656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="102500224"/>
+        <c:axId val="45877120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4008,7 +5391,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102539648"/>
+        <c:crossAx val="45878656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4016,7 +5399,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102539648"/>
+        <c:axId val="45878656"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4054,7 +5437,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102500224"/>
+        <c:crossAx val="45877120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4171,11 +5554,6 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3">
-                <a:lumMod val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
             <a:ln>
               <a:solidFill>
                 <a:schemeClr val="accent3">
@@ -4376,11 +5754,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="180618368"/>
-        <c:axId val="180683520"/>
+        <c:axId val="45920256"/>
+        <c:axId val="45922176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="180618368"/>
+        <c:axId val="45920256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4402,14 +5780,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="180683520"/>
+        <c:crossAx val="45922176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4417,7 +5794,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="180683520"/>
+        <c:axId val="45922176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4440,14 +5817,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="180618368"/>
+        <c:crossAx val="45920256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4764,11 +6140,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="185072640"/>
-        <c:axId val="185129984"/>
+        <c:axId val="45931904"/>
+        <c:axId val="45970944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="185072640"/>
+        <c:axId val="45931904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4790,14 +6166,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185129984"/>
+        <c:crossAx val="45970944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4805,7 +6180,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="185129984"/>
+        <c:axId val="45970944"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4829,14 +6204,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185072640"/>
+        <c:crossAx val="45931904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5160,16 +6534,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5193,7 +6567,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4238625" y="457200"/>
+          <a:off x="6791325" y="419100"/>
           <a:ext cx="4286250" cy="2819400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5216,15 +6590,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:colOff>285749</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>352424</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5238,6 +6612,102 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>185738</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>90488</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>109538</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5905,14 +7375,14 @@
       </c>
     </row>
     <row r="3" spans="2:15">
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
     </row>
     <row r="4" spans="2:15">
       <c r="B4" t="s">
@@ -5993,11 +7463,11 @@
         <v>2.7083514760950971</v>
       </c>
       <c r="L5" s="10">
-        <f>$C5/E5</f>
+        <f t="shared" ref="L5:M8" si="0">$C5/E5</f>
         <v>8.7139254693191379</v>
       </c>
       <c r="M5" s="10">
-        <f>$C5/F5</f>
+        <f t="shared" si="0"/>
         <v>10.636114911080712</v>
       </c>
       <c r="N5" s="4">
@@ -6047,15 +7517,15 @@
         <v>2.7465006402614032</v>
       </c>
       <c r="L6" s="10">
-        <f>$C6/E6</f>
+        <f t="shared" si="0"/>
         <v>8.6823003908431051</v>
       </c>
       <c r="M6" s="10">
-        <f>$C6/F6</f>
+        <f t="shared" si="0"/>
         <v>10.714900947459087</v>
       </c>
       <c r="N6" s="4">
-        <f t="shared" ref="N6:N8" si="0">C6/G6</f>
+        <f t="shared" ref="N6:N8" si="1">C6/G6</f>
         <v>230.37037037037035</v>
       </c>
       <c r="O6" s="4">
@@ -6101,15 +7571,15 @@
         <v>2.8446634561541049</v>
       </c>
       <c r="L7" s="10">
-        <f>$C7/E7</f>
+        <f t="shared" si="0"/>
         <v>8.8544934811406257</v>
       </c>
       <c r="M7" s="10">
-        <f>$C7/F7</f>
+        <f t="shared" si="0"/>
         <v>10.993767313019392</v>
       </c>
       <c r="N7" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>254</v>
       </c>
       <c r="O7" s="4">
@@ -6155,15 +7625,15 @@
         <v>2.8250106413961511</v>
       </c>
       <c r="L8" s="10">
-        <f>$C8/E8</f>
+        <f t="shared" si="0"/>
         <v>8.789600250932283</v>
       </c>
       <c r="M8" s="10">
-        <f>$C8/F8</f>
+        <f t="shared" si="0"/>
         <v>10.941906373378455</v>
       </c>
       <c r="N8" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>252.2</v>
       </c>
       <c r="O8" s="4">
@@ -6239,14 +7709,14 @@
       <c r="D13" t="s">
         <v>5</v>
       </c>
-      <c r="J13" s="14" t="s">
+      <c r="J13" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
     </row>
     <row r="14" spans="2:15">
       <c r="C14" t="s">
@@ -6309,34 +7779,34 @@
         <v>8000</v>
       </c>
       <c r="D16" s="4">
-        <f t="shared" ref="D16:D19" si="1">1/C16*1000000</f>
+        <f t="shared" ref="D16:D19" si="2">1/C16*1000000</f>
         <v>125</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>84</v>
       </c>
       <c r="J16" s="4">
-        <f>J15/$J15</f>
+        <f t="shared" ref="J16:O16" si="3">J15/$J15</f>
         <v>1</v>
       </c>
       <c r="K16" s="4">
-        <f>K15/$J15</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="L16" s="4">
-        <f>L15/$J15</f>
+        <f t="shared" si="3"/>
         <v>5.25</v>
       </c>
       <c r="M16" s="4">
-        <f>M15/$J15</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="N16" s="4">
-        <f>N15/$J15</f>
+        <f t="shared" si="3"/>
         <v>11.25</v>
       </c>
       <c r="O16" s="4">
-        <f>O15/$J15</f>
+        <f t="shared" si="3"/>
         <v>158.125</v>
       </c>
     </row>
@@ -6345,34 +7815,34 @@
         <v>11025</v>
       </c>
       <c r="D17" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>90.702947845804985</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="J17" s="15">
+      <c r="J17" s="14">
         <f>J8/J16</f>
         <v>1</v>
       </c>
-      <c r="K17" s="15">
-        <f t="shared" ref="K17:O17" si="2">K8/K16</f>
+      <c r="K17" s="14">
+        <f t="shared" ref="K17:O17" si="4">K8/K16</f>
         <v>0.94167021379871707</v>
       </c>
-      <c r="L17" s="15">
-        <f t="shared" si="2"/>
+      <c r="L17" s="14">
+        <f t="shared" si="4"/>
         <v>1.6742095716061491</v>
       </c>
-      <c r="M17" s="15">
-        <f t="shared" si="2"/>
+      <c r="M17" s="14">
+        <f t="shared" si="4"/>
         <v>1.8236510622297424</v>
       </c>
-      <c r="N17" s="15">
-        <f t="shared" si="2"/>
+      <c r="N17" s="14">
+        <f t="shared" si="4"/>
         <v>22.417777777777776</v>
       </c>
-      <c r="O17" s="15">
-        <f t="shared" si="2"/>
+      <c r="O17" s="14">
+        <f t="shared" si="4"/>
         <v>1.8188399035949943</v>
       </c>
     </row>
@@ -6381,7 +7851,7 @@
         <v>22050</v>
       </c>
       <c r="D18" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>45.351473922902493</v>
       </c>
       <c r="E18" s="4"/>
@@ -6399,7 +7869,7 @@
         <v>44100</v>
       </c>
       <c r="D19" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22.675736961451246</v>
       </c>
       <c r="E19" s="4"/>
@@ -6474,15 +7944,15 @@
         <v>#REF!</v>
       </c>
       <c r="V21" t="str">
-        <f t="shared" ref="V21:X21" si="3">E21</f>
+        <f t="shared" ref="V21:X21" si="5">E21</f>
         <v>Arduino Due</v>
       </c>
       <c r="W21" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Teensy 3.1</v>
       </c>
       <c r="X21" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>FRDM-K66F</v>
       </c>
     </row>
@@ -6604,11 +8074,11 @@
         <v>5.5045000000000002</v>
       </c>
       <c r="J24">
-        <f>C24/C24</f>
+        <f t="shared" ref="J24:J35" si="6">C24/C24</f>
         <v>1</v>
       </c>
       <c r="K24" s="6">
-        <f>C24/D24</f>
+        <f t="shared" ref="K24:K35" si="7">C24/D24</f>
         <v>2.7083514760950971</v>
       </c>
       <c r="L24" s="6">
@@ -6620,7 +8090,7 @@
         <v>10.636114911080712</v>
       </c>
       <c r="N24" s="6">
-        <f>C24/G24</f>
+        <f t="shared" ref="N24:N35" si="8">C24/G24</f>
         <v>239.23076923076923</v>
       </c>
       <c r="O24" s="6">
@@ -6634,11 +8104,11 @@
       </c>
       <c r="R24" s="6"/>
       <c r="S24" s="6">
-        <f>C24/C32</f>
+        <f t="shared" ref="S24:T27" si="9">C24/C32</f>
         <v>7.5853658536585362</v>
       </c>
       <c r="T24" s="6">
-        <f>D24/D32</f>
+        <f t="shared" si="9"/>
         <v>12.604829857299672</v>
       </c>
       <c r="U24" s="6" t="e">
@@ -6646,15 +8116,15 @@
         <v>#REF!</v>
       </c>
       <c r="V24" s="6">
-        <f t="shared" ref="V24:X24" si="4">E24/E32</f>
+        <f t="shared" ref="V24:X24" si="10">E24/E32</f>
         <v>5.499229583975346</v>
       </c>
       <c r="W24" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>13.537037037037035</v>
       </c>
       <c r="X24" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>0.92857142857142871</v>
       </c>
     </row>
@@ -6664,7 +8134,7 @@
         <v>32</v>
       </c>
       <c r="C25" s="4">
-        <f t="shared" ref="C25:C27" si="5">C6</f>
+        <f t="shared" ref="C25:C27" si="11">C6</f>
         <v>622</v>
       </c>
       <c r="D25" s="4">
@@ -6684,45 +8154,45 @@
         <v>2.7</v>
       </c>
       <c r="H25" s="10">
-        <f t="shared" ref="H25:H27" si="6">H6</f>
+        <f t="shared" ref="H25:H27" si="12">H6</f>
         <v>5.6927500000000002</v>
       </c>
       <c r="J25">
-        <f>C25/C25</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K25" s="6">
-        <f>C25/D25</f>
+        <f t="shared" si="7"/>
         <v>2.7465006402614032</v>
       </c>
       <c r="L25" s="6">
-        <f t="shared" ref="L25:L35" si="7">$C25/E25</f>
+        <f t="shared" ref="L25:L35" si="13">$C25/E25</f>
         <v>8.6823003908431051</v>
       </c>
       <c r="M25" s="6">
-        <f t="shared" ref="M25:M35" si="8">$C25/F25</f>
+        <f t="shared" ref="M25:M35" si="14">$C25/F25</f>
         <v>10.714900947459087</v>
       </c>
       <c r="N25" s="6">
-        <f>C25/G25</f>
+        <f t="shared" si="8"/>
         <v>230.37037037037035</v>
       </c>
       <c r="O25" s="6">
-        <f t="shared" ref="O25:O35" si="9">$C25/H25</f>
+        <f t="shared" ref="O25:O35" si="15">$C25/H25</f>
         <v>109.26178033463616</v>
       </c>
       <c r="P25" s="6"/>
       <c r="Q25" s="6">
-        <f t="shared" ref="Q25:Q35" si="10">F25/G25</f>
+        <f t="shared" ref="Q25:Q35" si="16">F25/G25</f>
         <v>21.499999999999996</v>
       </c>
       <c r="R25" s="6"/>
       <c r="S25" s="6">
-        <f>C25/C33</f>
+        <f t="shared" si="9"/>
         <v>7.8734177215189876</v>
       </c>
       <c r="T25" s="6">
-        <f>D25/D33</f>
+        <f t="shared" si="9"/>
         <v>12.970790378006873</v>
       </c>
       <c r="U25" s="6" t="e">
@@ -6730,15 +8200,15 @@
         <v>#REF!</v>
       </c>
       <c r="V25" s="6">
-        <f t="shared" ref="V25:V27" si="11">E25/E33</f>
+        <f t="shared" ref="V25:V27" si="17">E25/E33</f>
         <v>5.6857142857142859</v>
       </c>
       <c r="W25" s="6">
-        <f t="shared" ref="W25:X27" si="12">F25/F33</f>
+        <f t="shared" ref="W25:X27" si="18">F25/F33</f>
         <v>13.954326923076922</v>
       </c>
       <c r="X25" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0.96428571428571441</v>
       </c>
     </row>
@@ -6748,7 +8218,7 @@
         <v>64</v>
       </c>
       <c r="C26" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1270</v>
       </c>
       <c r="D26" s="4">
@@ -6768,45 +8238,45 @@
         <v>5</v>
       </c>
       <c r="H26" s="10">
+        <f t="shared" si="12"/>
+        <v>8.3607499999999995</v>
+      </c>
+      <c r="J26">
         <f t="shared" si="6"/>
-        <v>8.3607499999999995</v>
-      </c>
-      <c r="J26">
-        <f>C26/C26</f>
         <v>1</v>
       </c>
       <c r="K26" s="6">
-        <f>C26/D26</f>
+        <f t="shared" si="7"/>
         <v>2.8446634561541049</v>
       </c>
       <c r="L26" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>8.8544934811406257</v>
       </c>
       <c r="M26" s="6">
+        <f t="shared" si="14"/>
+        <v>10.993767313019392</v>
+      </c>
+      <c r="N26" s="6">
         <f t="shared" si="8"/>
-        <v>10.993767313019392</v>
-      </c>
-      <c r="N26" s="6">
-        <f>C26/G26</f>
         <v>254</v>
       </c>
       <c r="O26" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>151.90024818347638</v>
       </c>
       <c r="P26" s="6"/>
       <c r="Q26" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>23.103999999999999</v>
       </c>
       <c r="R26" s="6"/>
       <c r="S26" s="6">
-        <f>C26/C34</f>
+        <f t="shared" si="9"/>
         <v>8.193548387096774</v>
       </c>
       <c r="T26" s="6">
-        <f>D26/D34</f>
+        <f t="shared" si="9"/>
         <v>13.07320644216691</v>
       </c>
       <c r="U26" s="6" t="e">
@@ -6814,15 +8284,15 @@
         <v>#REF!</v>
       </c>
       <c r="V26" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>5.7834677419354836</v>
       </c>
       <c r="W26" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>14.13953488372093</v>
       </c>
       <c r="X26" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0.92592592592592582</v>
       </c>
     </row>
@@ -6832,7 +8302,7 @@
         <v>128</v>
       </c>
       <c r="C27" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>2522</v>
       </c>
       <c r="D27" s="4">
@@ -6852,45 +8322,45 @@
         <v>10</v>
       </c>
       <c r="H27" s="10">
+        <f t="shared" si="12"/>
+        <v>8.7690000000000001</v>
+      </c>
+      <c r="J27">
         <f t="shared" si="6"/>
-        <v>8.7690000000000001</v>
-      </c>
-      <c r="J27">
-        <f>C27/C27</f>
         <v>1</v>
       </c>
       <c r="K27" s="6">
-        <f>C27/D27</f>
+        <f t="shared" si="7"/>
         <v>2.8250106413961511</v>
       </c>
       <c r="L27" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>8.789600250932283</v>
       </c>
       <c r="M27" s="6">
+        <f t="shared" si="14"/>
+        <v>10.941906373378455</v>
+      </c>
+      <c r="N27" s="6">
         <f t="shared" si="8"/>
-        <v>10.941906373378455</v>
-      </c>
-      <c r="N27" s="6">
-        <f>C27/G27</f>
         <v>252.2</v>
       </c>
       <c r="O27" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>287.60405975595847</v>
       </c>
       <c r="P27" s="6"/>
       <c r="Q27" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>23.048999999999999</v>
       </c>
       <c r="R27" s="6"/>
       <c r="S27" s="6">
-        <f>C27/C35</f>
+        <f t="shared" si="9"/>
         <v>8.1883116883116891</v>
       </c>
       <c r="T27" s="6">
-        <f>D27/D35</f>
+        <f t="shared" si="9"/>
         <v>13.215988156920799</v>
       </c>
       <c r="U27" s="6" t="e">
@@ -6898,15 +8368,15 @@
         <v>#REF!</v>
       </c>
       <c r="V27" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>5.83072546230441</v>
       </c>
       <c r="W27" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>14.22777777777778</v>
       </c>
       <c r="X27" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0.93457943925233655</v>
       </c>
     </row>
@@ -6943,41 +8413,41 @@
         <v>5.5045000000000002</v>
       </c>
       <c r="J28">
-        <f>C28/C28</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K28" s="6">
-        <f>C28/D28</f>
+        <f t="shared" si="7"/>
         <v>11.977715877437326</v>
       </c>
       <c r="L28" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>19.876733436055471</v>
       </c>
       <c r="M28" s="6">
+        <f t="shared" si="14"/>
+        <v>59.722222222222221</v>
+      </c>
+      <c r="N28" s="6">
         <f t="shared" si="8"/>
-        <v>59.722222222222221</v>
-      </c>
-      <c r="N28" s="6">
-        <f>C28/G28</f>
         <v>92.142857142857153</v>
       </c>
       <c r="O28" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>23.435371060041785</v>
       </c>
       <c r="P28" s="6"/>
       <c r="Q28" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1.5428571428571431</v>
       </c>
       <c r="R28" s="6"/>
       <c r="S28" s="6">
-        <f>C28/C32</f>
+        <f t="shared" ref="S28:T31" si="19">C28/C32</f>
         <v>3.1463414634146343</v>
       </c>
       <c r="T28" s="6">
-        <f>D28/D32</f>
+        <f t="shared" si="19"/>
         <v>1.1822173435784853</v>
       </c>
       <c r="U28" s="6" t="e">
@@ -6985,21 +8455,21 @@
         <v>#REF!</v>
       </c>
       <c r="V28" s="6">
-        <f t="shared" ref="V28:X28" si="13">E28/E32</f>
+        <f t="shared" ref="V28:X28" si="20">E28/E32</f>
         <v>1</v>
       </c>
       <c r="W28" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="X28" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:24">
       <c r="B29">
-        <f t="shared" ref="B29:B35" si="14">B25</f>
+        <f t="shared" ref="B29:B35" si="21">B25</f>
         <v>32</v>
       </c>
       <c r="C29" s="4">
@@ -7019,49 +8489,49 @@
         <v>4.16</v>
       </c>
       <c r="G29" s="10">
-        <f t="shared" ref="G29:G31" si="15">G33</f>
+        <f t="shared" ref="G29:G31" si="22">G33</f>
         <v>2.8</v>
       </c>
       <c r="H29" s="10">
-        <f t="shared" ref="H29:H31" si="16">H25</f>
+        <f t="shared" ref="H29:H31" si="23">H25</f>
         <v>5.6927500000000002</v>
       </c>
       <c r="J29">
-        <f>C29/C29</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K29" s="6">
-        <f>C29/D29</f>
+        <f t="shared" si="7"/>
         <v>12.217412217412218</v>
       </c>
       <c r="L29" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>20.158730158730158</v>
       </c>
       <c r="M29" s="6">
+        <f t="shared" si="14"/>
+        <v>61.057692307692307</v>
+      </c>
+      <c r="N29" s="6">
         <f t="shared" si="8"/>
-        <v>61.057692307692307</v>
-      </c>
-      <c r="N29" s="6">
-        <f>C29/G29</f>
         <v>90.714285714285722</v>
       </c>
       <c r="O29" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>44.618154670414121</v>
       </c>
       <c r="P29" s="6"/>
       <c r="Q29" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1.4857142857142858</v>
       </c>
       <c r="R29" s="6"/>
       <c r="S29" s="6">
-        <f>C29/C33</f>
+        <f t="shared" si="19"/>
         <v>3.2151898734177213</v>
       </c>
       <c r="T29" s="6">
-        <f>D29/D33</f>
+        <f t="shared" si="19"/>
         <v>1.1907216494845361</v>
       </c>
       <c r="U29" s="6" t="e">
@@ -7069,21 +8539,21 @@
         <v>#REF!</v>
       </c>
       <c r="V29" s="6">
-        <f t="shared" ref="V29:V31" si="17">E29/E33</f>
+        <f t="shared" ref="V29:V31" si="24">E29/E33</f>
         <v>1</v>
       </c>
       <c r="W29" s="6">
-        <f t="shared" ref="W29:X31" si="18">F29/F33</f>
+        <f t="shared" ref="W29:X31" si="25">F29/F33</f>
         <v>1</v>
       </c>
       <c r="X29" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:24">
       <c r="B30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>64</v>
       </c>
       <c r="C30" s="4">
@@ -7103,49 +8573,49 @@
         <v>8.17</v>
       </c>
       <c r="G30" s="10">
+        <f t="shared" si="22"/>
+        <v>5.4</v>
+      </c>
+      <c r="H30" s="10">
+        <f t="shared" si="23"/>
+        <v>8.3607499999999995</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="K30" s="6">
+        <f t="shared" si="7"/>
+        <v>12.319373010041637</v>
+      </c>
+      <c r="L30" s="6">
+        <f t="shared" si="13"/>
+        <v>20.282258064516128</v>
+      </c>
+      <c r="M30" s="6">
+        <f t="shared" si="14"/>
+        <v>61.566707466340269</v>
+      </c>
+      <c r="N30" s="6">
+        <f t="shared" si="8"/>
+        <v>93.148148148148138</v>
+      </c>
+      <c r="O30" s="6">
         <f t="shared" si="15"/>
-        <v>5.4</v>
-      </c>
-      <c r="H30" s="10">
-        <f t="shared" si="16"/>
-        <v>8.3607499999999995</v>
-      </c>
-      <c r="J30">
-        <f>C30/C30</f>
-        <v>1</v>
-      </c>
-      <c r="K30" s="6">
-        <f>C30/D30</f>
-        <v>12.319373010041637</v>
-      </c>
-      <c r="L30" s="6">
-        <f t="shared" si="7"/>
-        <v>20.282258064516128</v>
-      </c>
-      <c r="M30" s="6">
-        <f t="shared" si="8"/>
-        <v>61.566707466340269</v>
-      </c>
-      <c r="N30" s="6">
-        <f>C30/G30</f>
-        <v>93.148148148148138</v>
-      </c>
-      <c r="O30" s="6">
-        <f t="shared" si="9"/>
         <v>60.162066800227258</v>
       </c>
       <c r="P30" s="6"/>
       <c r="Q30" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1.5129629629629628</v>
       </c>
       <c r="R30" s="6"/>
       <c r="S30" s="6">
-        <f>C30/C34</f>
+        <f t="shared" si="19"/>
         <v>3.2451612903225806</v>
       </c>
       <c r="T30" s="6">
-        <f>D30/D34</f>
+        <f t="shared" si="19"/>
         <v>1.1956076134699853</v>
       </c>
       <c r="U30" s="6" t="e">
@@ -7153,21 +8623,21 @@
         <v>#REF!</v>
       </c>
       <c r="V30" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="W30" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>1</v>
       </c>
       <c r="X30" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:24">
       <c r="B31">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>128</v>
       </c>
       <c r="C31" s="4">
@@ -7187,49 +8657,49 @@
         <v>16.2</v>
       </c>
       <c r="G31" s="10">
+        <f t="shared" si="22"/>
+        <v>10.7</v>
+      </c>
+      <c r="H31" s="10">
+        <f t="shared" si="23"/>
+        <v>8.7690000000000001</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="K31" s="6">
+        <f t="shared" si="7"/>
+        <v>12.384130515387469</v>
+      </c>
+      <c r="L31" s="6">
+        <f t="shared" si="13"/>
+        <v>20.361715098557202</v>
+      </c>
+      <c r="M31" s="6">
+        <f t="shared" si="14"/>
+        <v>61.851851851851855</v>
+      </c>
+      <c r="N31" s="6">
+        <f t="shared" si="8"/>
+        <v>93.644859813084125</v>
+      </c>
+      <c r="O31" s="6">
         <f t="shared" si="15"/>
-        <v>10.7</v>
-      </c>
-      <c r="H31" s="10">
-        <f t="shared" si="16"/>
-        <v>8.7690000000000001</v>
-      </c>
-      <c r="J31">
-        <f>C31/C31</f>
-        <v>1</v>
-      </c>
-      <c r="K31" s="6">
-        <f>C31/D31</f>
-        <v>12.384130515387469</v>
-      </c>
-      <c r="L31" s="6">
-        <f t="shared" si="7"/>
-        <v>20.361715098557202</v>
-      </c>
-      <c r="M31" s="6">
-        <f t="shared" si="8"/>
-        <v>61.851851851851855</v>
-      </c>
-      <c r="N31" s="6">
-        <f>C31/G31</f>
-        <v>93.644859813084125</v>
-      </c>
-      <c r="O31" s="6">
-        <f t="shared" si="9"/>
         <v>114.26616489907629</v>
       </c>
       <c r="P31" s="6"/>
       <c r="Q31" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1.514018691588785</v>
       </c>
       <c r="R31" s="6"/>
       <c r="S31" s="6">
-        <f>C31/C35</f>
+        <f t="shared" si="19"/>
         <v>3.2532467532467533</v>
       </c>
       <c r="T31" s="6">
-        <f>D31/D35</f>
+        <f t="shared" si="19"/>
         <v>1.197779422649889</v>
       </c>
       <c r="U31" s="6" t="e">
@@ -7237,15 +8707,15 @@
         <v>#REF!</v>
       </c>
       <c r="V31" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="W31" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>1</v>
       </c>
       <c r="X31" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>1</v>
       </c>
     </row>
@@ -7254,7 +8724,7 @@
         <v>64</v>
       </c>
       <c r="B32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>16</v>
       </c>
       <c r="C32" s="4">
@@ -7282,32 +8752,32 @@
         <v>5.5045000000000002</v>
       </c>
       <c r="J32">
-        <f>C32/C32</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K32" s="6">
-        <f>C32/D32</f>
+        <f t="shared" si="7"/>
         <v>4.5005488474204176</v>
       </c>
       <c r="L32" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>6.3174114021571643</v>
       </c>
       <c r="M32" s="6">
+        <f t="shared" si="14"/>
+        <v>18.981481481481481</v>
+      </c>
+      <c r="N32" s="6">
         <f t="shared" si="8"/>
-        <v>18.981481481481481</v>
-      </c>
-      <c r="N32" s="6">
-        <f>C32/G32</f>
         <v>29.285714285714288</v>
       </c>
       <c r="O32" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>7.4484512671450629</v>
       </c>
       <c r="P32" s="6"/>
       <c r="Q32" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1.5428571428571431</v>
       </c>
       <c r="R32" s="6"/>
@@ -7318,7 +8788,7 @@
     </row>
     <row r="33" spans="1:22">
       <c r="B33">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>32</v>
       </c>
       <c r="C33" s="4">
@@ -7334,7 +8804,7 @@
         <v>12.6</v>
       </c>
       <c r="F33">
-        <f t="shared" ref="F33:F35" si="19">F29</f>
+        <f t="shared" ref="F33:F35" si="26">F29</f>
         <v>4.16</v>
       </c>
       <c r="G33" s="10">
@@ -7342,36 +8812,36 @@
         <v>2.8</v>
       </c>
       <c r="H33" s="10">
-        <f t="shared" ref="H33:H35" si="20">H25</f>
+        <f t="shared" ref="H33:H35" si="27">H25</f>
         <v>5.6927500000000002</v>
       </c>
       <c r="J33">
-        <f>C33/C33</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K33" s="6">
-        <f>C33/D33</f>
+        <f t="shared" si="7"/>
         <v>4.5246277205040091</v>
       </c>
       <c r="L33" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>6.2698412698412698</v>
       </c>
       <c r="M33" s="6">
+        <f t="shared" si="14"/>
+        <v>18.990384615384613</v>
+      </c>
+      <c r="N33" s="6">
         <f t="shared" si="8"/>
-        <v>18.990384615384613</v>
-      </c>
-      <c r="N33" s="6">
-        <f>C33/G33</f>
         <v>28.214285714285715</v>
       </c>
       <c r="O33" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>13.877300074656361</v>
       </c>
       <c r="P33" s="6"/>
       <c r="Q33" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1.4857142857142858</v>
       </c>
       <c r="R33" s="6"/>
@@ -7398,7 +8868,7 @@
         <v>24.8</v>
       </c>
       <c r="F34">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>8.17</v>
       </c>
       <c r="G34" s="10">
@@ -7406,36 +8876,36 @@
         <v>5.4</v>
       </c>
       <c r="H34" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v>8.3607499999999995</v>
       </c>
       <c r="J34">
-        <f>C34/C34</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K34" s="6">
-        <f>C34/D34</f>
+        <f t="shared" si="7"/>
         <v>4.5387994143484631</v>
       </c>
       <c r="L34" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>6.25</v>
       </c>
       <c r="M34" s="6">
+        <f t="shared" si="14"/>
+        <v>18.971848225214199</v>
+      </c>
+      <c r="N34" s="6">
         <f t="shared" si="8"/>
-        <v>18.971848225214199</v>
-      </c>
-      <c r="N34" s="6">
-        <f>C34/G34</f>
         <v>28.703703703703702</v>
       </c>
       <c r="O34" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>18.539006668062076</v>
       </c>
       <c r="P34" s="6"/>
       <c r="Q34" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1.5129629629629628</v>
       </c>
       <c r="R34" s="6"/>
@@ -7446,7 +8916,7 @@
     </row>
     <row r="35" spans="1:22">
       <c r="B35">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>128</v>
       </c>
       <c r="C35" s="4">
@@ -7462,7 +8932,7 @@
         <v>49.21</v>
       </c>
       <c r="F35">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>16.2</v>
       </c>
       <c r="G35" s="10">
@@ -7470,36 +8940,36 @@
         <v>10.7</v>
       </c>
       <c r="H35" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v>8.7690000000000001</v>
       </c>
       <c r="J35">
-        <f>C35/C35</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K35" s="6">
-        <f>C35/D35</f>
+        <f t="shared" si="7"/>
         <v>4.5595854922279795</v>
       </c>
       <c r="L35" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>6.2588904694167855</v>
       </c>
       <c r="M35" s="6">
+        <f t="shared" si="14"/>
+        <v>19.012345679012345</v>
+      </c>
+      <c r="N35" s="6">
         <f t="shared" si="8"/>
-        <v>19.012345679012345</v>
-      </c>
-      <c r="N35" s="6">
-        <f>C35/G35</f>
         <v>28.785046728971963</v>
       </c>
       <c r="O35" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>35.12373132626297</v>
       </c>
       <c r="P35" s="6"/>
       <c r="Q35" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1.514018691588785</v>
       </c>
       <c r="R35" s="6"/>
@@ -7521,19 +8991,19 @@
         <v>1607.7170418006433</v>
       </c>
       <c r="D37" s="8">
-        <f t="shared" ref="D37:F37" si="21">1/(D25*0.000001)</f>
+        <f t="shared" ref="D37:F37" si="28">1/(D25*0.000001)</f>
         <v>4415.5958846646354</v>
       </c>
       <c r="E37" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>13958.682300390843</v>
       </c>
       <c r="F37" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>17226.528854435834</v>
       </c>
       <c r="G37" s="8">
-        <f t="shared" ref="G37" si="22">1/(G25*0.000001)</f>
+        <f t="shared" ref="G37" si="29">1/(G25*0.000001)</f>
         <v>370370.37037037039</v>
       </c>
       <c r="H37" s="8">
@@ -7552,15 +9022,15 @@
         <v>0.3471833351999104</v>
       </c>
       <c r="L37" s="9">
-        <f t="shared" ref="L37:N37" si="23">$C$34/E26</f>
+        <f t="shared" ref="L37:N37" si="30">$C$34/E26</f>
         <v>1.0806665272258245</v>
       </c>
       <c r="M37" s="9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v>1.3417590027700832</v>
       </c>
       <c r="N37" s="9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v>31</v>
       </c>
       <c r="O37" s="9">
@@ -7581,23 +9051,23 @@
         <v>3937.0078740157483</v>
       </c>
       <c r="D38" s="8">
-        <f t="shared" ref="D38:F38" si="24">1/(D29*0.000001)</f>
+        <f t="shared" ref="D38:F38" si="31">1/(D29*0.000001)</f>
         <v>48100.048100048101</v>
       </c>
       <c r="E38" s="8">
-        <f t="shared" si="24"/>
+        <f t="shared" si="31"/>
         <v>79365.079365079364</v>
       </c>
       <c r="F38" s="8">
-        <f t="shared" si="24"/>
+        <f t="shared" si="31"/>
         <v>240384.61538461538</v>
       </c>
       <c r="G38" s="8">
-        <f t="shared" ref="G38" si="25">1/(G29*0.000001)</f>
+        <f t="shared" ref="G38" si="32">1/(G29*0.000001)</f>
         <v>357142.85714285716</v>
       </c>
       <c r="H38" s="8">
-        <f t="shared" ref="H38" si="26">1/(H29*0.000001)</f>
+        <f t="shared" ref="H38" si="33">1/(H29*0.000001)</f>
         <v>175662.02626147293</v>
       </c>
       <c r="I38" t="s">
@@ -7612,15 +9082,15 @@
         <v>3.7962282635317171</v>
       </c>
       <c r="L38" s="9">
-        <f t="shared" ref="L38:N38" si="27">$C$34/E30</f>
+        <f t="shared" ref="L38:N38" si="34">$C$34/E30</f>
         <v>6.25</v>
       </c>
       <c r="M38" s="9">
-        <f t="shared" si="27"/>
+        <f t="shared" si="34"/>
         <v>18.971848225214199</v>
       </c>
       <c r="N38" s="9">
-        <f t="shared" si="27"/>
+        <f t="shared" si="34"/>
         <v>28.703703703703702</v>
       </c>
       <c r="O38" s="9">
@@ -7641,23 +9111,23 @@
         <v>12658.227848101267</v>
       </c>
       <c r="D39" s="8">
-        <f t="shared" ref="D39:F39" si="28">1/(D33*0.000001)</f>
+        <f t="shared" ref="D39:F39" si="35">1/(D33*0.000001)</f>
         <v>57273.768613974804</v>
       </c>
       <c r="E39" s="8">
-        <f t="shared" si="28"/>
+        <f t="shared" si="35"/>
         <v>79365.079365079364</v>
       </c>
       <c r="F39" s="8">
-        <f t="shared" si="28"/>
+        <f t="shared" si="35"/>
         <v>240384.61538461538</v>
       </c>
       <c r="G39" s="8">
-        <f t="shared" ref="G39" si="29">1/(G33*0.000001)</f>
+        <f t="shared" ref="G39" si="36">1/(G33*0.000001)</f>
         <v>357142.85714285716</v>
       </c>
       <c r="H39" s="8">
-        <f t="shared" ref="H39" si="30">1/(H33*0.000001)</f>
+        <f t="shared" ref="H39" si="37">1/(H33*0.000001)</f>
         <v>175662.02626147293</v>
       </c>
       <c r="I39" t="s">
@@ -7672,15 +9142,15 @@
         <v>4.5387994143484631</v>
       </c>
       <c r="L39" s="9">
-        <f t="shared" ref="L39:N39" si="31">$C$34/E34</f>
+        <f t="shared" ref="L39:N39" si="38">$C$34/E34</f>
         <v>6.25</v>
       </c>
       <c r="M39" s="9">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>18.971848225214199</v>
       </c>
       <c r="N39" s="9">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>28.703703703703702</v>
       </c>
       <c r="O39" s="9">
@@ -7701,27 +9171,27 @@
     </row>
     <row r="58" spans="2:9">
       <c r="C58">
-        <f>C$21</f>
+        <f t="shared" ref="C58:H58" si="39">C$21</f>
         <v>0</v>
       </c>
       <c r="D58" t="str">
-        <f>D$21</f>
+        <f t="shared" si="39"/>
         <v>Arduino M0</v>
       </c>
       <c r="E58" t="str">
-        <f>E$21</f>
+        <f t="shared" si="39"/>
         <v>Arduino Due</v>
       </c>
       <c r="F58" t="str">
-        <f>F$21</f>
+        <f t="shared" si="39"/>
         <v>Teensy 3.1</v>
       </c>
       <c r="G58" t="str">
-        <f>G$21</f>
+        <f t="shared" si="39"/>
         <v>FRDM-K66F</v>
       </c>
       <c r="H58" t="str">
-        <f>H$21</f>
+        <f t="shared" si="39"/>
         <v>Python, PC</v>
       </c>
     </row>
@@ -7867,7 +9337,7 @@
     </row>
     <row r="82" spans="1:8">
       <c r="B82" t="str">
-        <f>B23</f>
+        <f t="shared" ref="B82:B94" si="40">B23</f>
         <v>N_FIR</v>
       </c>
       <c r="C82" t="s">
@@ -7892,108 +9362,108 @@
         <v>float</v>
       </c>
       <c r="B83">
-        <f>B24</f>
+        <f t="shared" si="40"/>
         <v>16</v>
       </c>
       <c r="C83" s="11">
-        <f>1000000/C24</f>
+        <f t="shared" ref="C83:G94" si="41">1000000/C24</f>
         <v>3215.4340836012861</v>
       </c>
       <c r="D83" s="11">
-        <f>1000000/D24</f>
+        <f t="shared" si="41"/>
         <v>8708.52564660803</v>
       </c>
       <c r="E83" s="11">
-        <f>1000000/E24</f>
+        <f t="shared" si="41"/>
         <v>28019.052956010088</v>
       </c>
       <c r="F83" s="11">
-        <f>1000000/F24</f>
+        <f t="shared" si="41"/>
         <v>34199.726402188782</v>
       </c>
       <c r="G83" s="11">
-        <f>1000000/G24</f>
+        <f t="shared" si="41"/>
         <v>769230.76923076925</v>
       </c>
       <c r="H83" s="11"/>
     </row>
     <row r="84" spans="1:8">
       <c r="B84">
-        <f>B25</f>
+        <f t="shared" si="40"/>
         <v>32</v>
       </c>
       <c r="C84" s="11">
-        <f>1000000/C25</f>
+        <f t="shared" si="41"/>
         <v>1607.7170418006431</v>
       </c>
       <c r="D84" s="11">
-        <f>1000000/D25</f>
+        <f t="shared" si="41"/>
         <v>4415.5958846646354</v>
       </c>
       <c r="E84" s="11">
-        <f>1000000/E25</f>
+        <f t="shared" si="41"/>
         <v>13958.682300390843</v>
       </c>
       <c r="F84" s="11">
-        <f>1000000/F25</f>
+        <f t="shared" si="41"/>
         <v>17226.528854435834</v>
       </c>
       <c r="G84" s="11">
-        <f>1000000/G25</f>
+        <f t="shared" si="41"/>
         <v>370370.37037037034</v>
       </c>
       <c r="H84" s="11"/>
     </row>
     <row r="85" spans="1:8">
       <c r="B85">
-        <f>B26</f>
+        <f t="shared" si="40"/>
         <v>64</v>
       </c>
       <c r="C85" s="11">
-        <f>1000000/C26</f>
+        <f t="shared" si="41"/>
         <v>787.40157480314963</v>
       </c>
       <c r="D85" s="11">
-        <f>1000000/D26</f>
+        <f t="shared" si="41"/>
         <v>2239.8924851607126</v>
       </c>
       <c r="E85" s="11">
-        <f>1000000/E26</f>
+        <f t="shared" si="41"/>
         <v>6972.0421111343512</v>
       </c>
       <c r="F85" s="11">
-        <f>1000000/F26</f>
+        <f t="shared" si="41"/>
         <v>8656.5096952908589</v>
       </c>
       <c r="G85" s="11">
-        <f>1000000/G26</f>
+        <f t="shared" si="41"/>
         <v>200000</v>
       </c>
       <c r="H85" s="11"/>
     </row>
     <row r="86" spans="1:8">
       <c r="B86">
-        <f>B27</f>
+        <f t="shared" si="40"/>
         <v>128</v>
       </c>
       <c r="C86" s="11">
-        <f>1000000/C27</f>
+        <f t="shared" si="41"/>
         <v>396.51070578905632</v>
       </c>
       <c r="D86" s="11">
-        <f>1000000/D27</f>
+        <f t="shared" si="41"/>
         <v>1120.1469632815824</v>
       </c>
       <c r="E86" s="11">
-        <f>1000000/E27</f>
+        <f t="shared" si="41"/>
         <v>3485.1705991008257</v>
       </c>
       <c r="F86" s="11">
-        <f>1000000/F27</f>
+        <f t="shared" si="41"/>
         <v>4338.5830187860647</v>
       </c>
       <c r="G86" s="11">
-        <f>1000000/G27</f>
+        <f t="shared" si="41"/>
         <v>100000</v>
       </c>
       <c r="H86" s="11"/>
@@ -8004,108 +9474,108 @@
         <v>int32</v>
       </c>
       <c r="B87">
-        <f>B28</f>
+        <f t="shared" si="40"/>
         <v>16</v>
       </c>
       <c r="C87" s="11">
-        <f>1000000/C28</f>
+        <f t="shared" si="41"/>
         <v>7751.937984496124</v>
       </c>
       <c r="D87" s="11">
-        <f>1000000/D28</f>
+        <f t="shared" si="41"/>
         <v>92850.510677808736</v>
       </c>
       <c r="E87" s="11">
-        <f>1000000/E28</f>
+        <f t="shared" si="41"/>
         <v>154083.20493066256</v>
       </c>
       <c r="F87" s="11">
-        <f>1000000/F28</f>
+        <f t="shared" si="41"/>
         <v>462962.96296296292</v>
       </c>
       <c r="G87" s="11">
-        <f>1000000/G28</f>
+        <f t="shared" si="41"/>
         <v>714285.71428571432</v>
       </c>
       <c r="H87" s="11"/>
     </row>
     <row r="88" spans="1:8">
       <c r="B88">
-        <f>B29</f>
+        <f t="shared" si="40"/>
         <v>32</v>
       </c>
       <c r="C88" s="11">
-        <f>1000000/C29</f>
+        <f t="shared" si="41"/>
         <v>3937.0078740157483</v>
       </c>
       <c r="D88" s="11">
-        <f>1000000/D29</f>
+        <f t="shared" si="41"/>
         <v>48100.048100048101</v>
       </c>
       <c r="E88" s="11">
-        <f>1000000/E29</f>
+        <f t="shared" si="41"/>
         <v>79365.079365079364</v>
       </c>
       <c r="F88" s="11">
-        <f>1000000/F29</f>
+        <f t="shared" si="41"/>
         <v>240384.61538461538</v>
       </c>
       <c r="G88" s="11">
-        <f>1000000/G29</f>
+        <f t="shared" si="41"/>
         <v>357142.85714285716</v>
       </c>
       <c r="H88" s="11"/>
     </row>
     <row r="89" spans="1:8">
       <c r="B89">
-        <f>B30</f>
+        <f t="shared" si="40"/>
         <v>64</v>
       </c>
       <c r="C89" s="11">
-        <f>1000000/C30</f>
+        <f t="shared" si="41"/>
         <v>1988.0715705765408</v>
       </c>
       <c r="D89" s="11">
-        <f>1000000/D30</f>
+        <f t="shared" si="41"/>
         <v>24491.795248591723</v>
       </c>
       <c r="E89" s="11">
-        <f>1000000/E30</f>
+        <f t="shared" si="41"/>
         <v>40322.580645161288</v>
       </c>
       <c r="F89" s="11">
-        <f>1000000/F30</f>
+        <f t="shared" si="41"/>
         <v>122399.02080783354</v>
       </c>
       <c r="G89" s="11">
-        <f>1000000/G30</f>
+        <f t="shared" si="41"/>
         <v>185185.18518518517</v>
       </c>
       <c r="H89" s="11"/>
     </row>
     <row r="90" spans="1:8">
       <c r="B90">
-        <f>B31</f>
+        <f t="shared" si="40"/>
         <v>128</v>
       </c>
       <c r="C90" s="11">
-        <f>1000000/C31</f>
+        <f t="shared" si="41"/>
         <v>998.00399201596804</v>
       </c>
       <c r="D90" s="11">
-        <f>1000000/D31</f>
+        <f t="shared" si="41"/>
         <v>12359.411692003461</v>
       </c>
       <c r="E90" s="11">
-        <f>1000000/E31</f>
+        <f t="shared" si="41"/>
         <v>20321.072952651899</v>
       </c>
       <c r="F90" s="11">
-        <f>1000000/F31</f>
+        <f t="shared" si="41"/>
         <v>61728.395061728399</v>
       </c>
       <c r="G90" s="11">
-        <f>1000000/G31</f>
+        <f t="shared" si="41"/>
         <v>93457.943925233645</v>
       </c>
       <c r="H90" s="11"/>
@@ -8116,108 +9586,108 @@
         <v>int16</v>
       </c>
       <c r="B91">
-        <f>B32</f>
+        <f t="shared" si="40"/>
         <v>16</v>
       </c>
       <c r="C91" s="11">
-        <f>1000000/C32</f>
+        <f t="shared" si="41"/>
         <v>24390.243902439026</v>
       </c>
       <c r="D91" s="11">
-        <f>1000000/D32</f>
+        <f t="shared" si="41"/>
         <v>109769.48408342482</v>
       </c>
       <c r="E91" s="11">
-        <f>1000000/E32</f>
+        <f t="shared" si="41"/>
         <v>154083.20493066256</v>
       </c>
       <c r="F91" s="11">
-        <f>1000000/F32</f>
+        <f t="shared" si="41"/>
         <v>462962.96296296292</v>
       </c>
       <c r="G91" s="11">
-        <f>1000000/G32</f>
+        <f t="shared" si="41"/>
         <v>714285.71428571432</v>
       </c>
       <c r="H91" s="11"/>
     </row>
     <row r="92" spans="1:8">
       <c r="B92">
-        <f>B33</f>
+        <f t="shared" si="40"/>
         <v>32</v>
       </c>
       <c r="C92" s="11">
-        <f>1000000/C33</f>
+        <f t="shared" si="41"/>
         <v>12658.227848101265</v>
       </c>
       <c r="D92" s="11">
-        <f>1000000/D33</f>
+        <f t="shared" si="41"/>
         <v>57273.768613974797</v>
       </c>
       <c r="E92" s="11">
-        <f>1000000/E33</f>
+        <f t="shared" si="41"/>
         <v>79365.079365079364</v>
       </c>
       <c r="F92" s="11">
-        <f>1000000/F33</f>
+        <f t="shared" si="41"/>
         <v>240384.61538461538</v>
       </c>
       <c r="G92" s="11">
-        <f>1000000/G33</f>
+        <f t="shared" si="41"/>
         <v>357142.85714285716</v>
       </c>
       <c r="H92" s="11"/>
     </row>
     <row r="93" spans="1:8">
       <c r="B93">
-        <f>B34</f>
+        <f t="shared" si="40"/>
         <v>64</v>
       </c>
       <c r="C93" s="11">
-        <f>1000000/C34</f>
+        <f t="shared" si="41"/>
         <v>6451.6129032258068</v>
       </c>
       <c r="D93" s="11">
-        <f>1000000/D34</f>
+        <f t="shared" si="41"/>
         <v>29282.576866764277</v>
       </c>
       <c r="E93" s="11">
-        <f>1000000/E34</f>
+        <f t="shared" si="41"/>
         <v>40322.580645161288</v>
       </c>
       <c r="F93" s="11">
-        <f>1000000/F34</f>
+        <f t="shared" si="41"/>
         <v>122399.02080783354</v>
       </c>
       <c r="G93" s="11">
-        <f>1000000/G34</f>
+        <f t="shared" si="41"/>
         <v>185185.18518518517</v>
       </c>
       <c r="H93" s="11"/>
     </row>
     <row r="94" spans="1:8">
       <c r="B94">
-        <f>B35</f>
+        <f t="shared" si="40"/>
         <v>128</v>
       </c>
       <c r="C94" s="11">
-        <f>1000000/C35</f>
+        <f t="shared" si="41"/>
         <v>3246.7532467532469</v>
       </c>
       <c r="D94" s="11">
-        <f>1000000/D35</f>
+        <f t="shared" si="41"/>
         <v>14803.849000740192</v>
       </c>
       <c r="E94" s="11">
-        <f>1000000/E35</f>
+        <f t="shared" si="41"/>
         <v>20321.072952651899</v>
       </c>
       <c r="F94" s="11">
-        <f>1000000/F35</f>
+        <f t="shared" si="41"/>
         <v>61728.395061728399</v>
       </c>
       <c r="G94" s="11">
-        <f>1000000/G35</f>
+        <f t="shared" si="41"/>
         <v>93457.943925233645</v>
       </c>
       <c r="H94" s="11"/>
@@ -8240,27 +9710,27 @@
     </row>
     <row r="99" spans="2:8">
       <c r="C99">
-        <f>C$21</f>
+        <f t="shared" ref="C99:H99" si="42">C$21</f>
         <v>0</v>
       </c>
       <c r="D99" t="str">
-        <f>D$21</f>
+        <f t="shared" si="42"/>
         <v>Arduino M0</v>
       </c>
       <c r="E99" t="str">
-        <f>E$21</f>
+        <f t="shared" si="42"/>
         <v>Arduino Due</v>
       </c>
       <c r="F99" t="str">
-        <f>F$21</f>
+        <f t="shared" si="42"/>
         <v>Teensy 3.1</v>
       </c>
       <c r="G99" t="str">
-        <f>G$21</f>
+        <f t="shared" si="42"/>
         <v>FRDM-K66F</v>
       </c>
       <c r="H99" t="str">
-        <f>H$21</f>
+        <f t="shared" si="42"/>
         <v>Python, PC</v>
       </c>
     </row>
@@ -8274,7 +9744,7 @@
         <v>1.9843749999999998E-5</v>
       </c>
       <c r="D100">
-        <f t="shared" ref="D100" si="32">D26*0.000001/$B26</f>
+        <f t="shared" ref="D100" si="43">D26*0.000001/$B26</f>
         <v>6.9757812499999997E-6</v>
       </c>
       <c r="E100">
@@ -8304,7 +9774,7 @@
         <v>7.8281249999999988E-6</v>
       </c>
       <c r="D101">
-        <f t="shared" ref="D101" si="33">D31*0.000001/$B31</f>
+        <f t="shared" ref="D101" si="44">D31*0.000001/$B31</f>
         <v>6.3210937499999997E-7</v>
       </c>
       <c r="E101">
@@ -8334,7 +9804,7 @@
         <v>2.40625E-6</v>
       </c>
       <c r="D102">
-        <f t="shared" ref="D102" si="34">D35*0.000001/$B35</f>
+        <f t="shared" ref="D102" si="45">D35*0.000001/$B35</f>
         <v>5.2773437499999991E-7</v>
       </c>
       <c r="E102">
@@ -8361,27 +9831,27 @@
     </row>
     <row r="105" spans="2:8">
       <c r="C105">
-        <f>C$21</f>
+        <f t="shared" ref="C105:H105" si="46">C$21</f>
         <v>0</v>
       </c>
       <c r="D105" t="str">
-        <f>D$21</f>
+        <f t="shared" si="46"/>
         <v>Arduino M0</v>
       </c>
       <c r="E105" t="str">
-        <f>E$21</f>
+        <f t="shared" si="46"/>
         <v>Arduino Due</v>
       </c>
       <c r="F105" t="str">
-        <f>F$21</f>
+        <f t="shared" si="46"/>
         <v>Teensy 3.1</v>
       </c>
       <c r="G105" t="str">
-        <f>G$21</f>
+        <f t="shared" si="46"/>
         <v>FRDM-K66F</v>
       </c>
       <c r="H105" t="str">
-        <f>H$21</f>
+        <f t="shared" si="46"/>
         <v>Python, PC</v>
       </c>
     </row>
@@ -8391,27 +9861,27 @@
         <v>float</v>
       </c>
       <c r="C106" s="10">
-        <f>(1/$G$96)/C100</f>
+        <f t="shared" ref="C106:H108" si="47">(1/$G$96)/C100</f>
         <v>1.5748031496062995</v>
       </c>
       <c r="D106" s="10">
-        <f>(1/$G$96)/D100</f>
+        <f t="shared" si="47"/>
         <v>4.4797849703214245</v>
       </c>
       <c r="E106" s="10">
-        <f>(1/$G$96)/E100</f>
+        <f t="shared" si="47"/>
         <v>13.944084222268703</v>
       </c>
       <c r="F106" s="10">
-        <f>(1/$G$96)/F100</f>
+        <f t="shared" si="47"/>
         <v>17.313019390581719</v>
       </c>
       <c r="G106" s="10">
-        <f>(1/$G$96)/G100</f>
+        <f t="shared" si="47"/>
         <v>400.00000000000006</v>
       </c>
       <c r="H106" s="10">
-        <f>(1/$G$96)/H100</f>
+        <f t="shared" si="47"/>
         <v>239.21298926531713</v>
       </c>
     </row>
@@ -8421,27 +9891,27 @@
         <v>int32</v>
       </c>
       <c r="C107" s="10">
-        <f>(1/$G$96)/C101</f>
+        <f t="shared" si="47"/>
         <v>3.9920159680638729</v>
       </c>
       <c r="D107" s="10">
-        <f>(1/$G$96)/D101</f>
+        <f t="shared" si="47"/>
         <v>49.437646768013849</v>
       </c>
       <c r="E107" s="10">
-        <f>(1/$G$96)/E101</f>
+        <f t="shared" si="47"/>
         <v>81.284291810607598</v>
       </c>
       <c r="F107" s="10">
-        <f>(1/$G$96)/F101</f>
+        <f t="shared" si="47"/>
         <v>246.91358024691363</v>
       </c>
       <c r="G107" s="10">
-        <f>(1/$G$96)/G101</f>
+        <f t="shared" si="47"/>
         <v>373.8317757009346</v>
       </c>
       <c r="H107" s="10">
-        <f>(1/$G$96)/H101</f>
+        <f t="shared" si="47"/>
         <v>456.15235488653212</v>
       </c>
     </row>
@@ -8451,27 +9921,27 @@
         <v>int16</v>
       </c>
       <c r="C108" s="10">
-        <f>(1/$G$96)/C102</f>
+        <f t="shared" si="47"/>
         <v>12.987012987012987</v>
       </c>
       <c r="D108" s="10">
-        <f>(1/$G$96)/D102</f>
+        <f t="shared" si="47"/>
         <v>59.21539600296078</v>
       </c>
       <c r="E108" s="10">
-        <f>(1/$G$96)/E102</f>
+        <f t="shared" si="47"/>
         <v>81.284291810607598</v>
       </c>
       <c r="F108" s="10">
-        <f>(1/$G$96)/F102</f>
+        <f t="shared" si="47"/>
         <v>246.91358024691363</v>
       </c>
       <c r="G108" s="10">
-        <f>(1/$G$96)/G102</f>
+        <f t="shared" si="47"/>
         <v>373.8317757009346</v>
       </c>
       <c r="H108" s="10">
-        <f>(1/$G$96)/H102</f>
+        <f t="shared" si="47"/>
         <v>456.15235488653212</v>
       </c>
     </row>
@@ -8482,27 +9952,27 @@
     </row>
     <row r="111" spans="2:8">
       <c r="C111">
-        <f>C$21</f>
+        <f t="shared" ref="C111:H111" si="48">C$21</f>
         <v>0</v>
       </c>
       <c r="D111" t="str">
-        <f>D$21</f>
+        <f t="shared" si="48"/>
         <v>Arduino M0</v>
       </c>
       <c r="E111" t="str">
-        <f>E$21</f>
+        <f t="shared" si="48"/>
         <v>Arduino Due</v>
       </c>
       <c r="F111" t="str">
-        <f>F$21</f>
+        <f t="shared" si="48"/>
         <v>Teensy 3.1</v>
       </c>
       <c r="G111" t="str">
-        <f>G$21</f>
+        <f t="shared" si="48"/>
         <v>FRDM-K66F</v>
       </c>
       <c r="H111" t="str">
-        <f>H$21</f>
+        <f t="shared" si="48"/>
         <v>Python, PC</v>
       </c>
     </row>
@@ -8512,27 +9982,27 @@
         <v>float</v>
       </c>
       <c r="C112" s="11">
-        <f>$G$96/C106</f>
+        <f t="shared" ref="C112:H114" si="49">$G$96/C106</f>
         <v>20319.999999999996</v>
       </c>
       <c r="D112" s="11">
-        <f>$G$96/D106</f>
+        <f t="shared" si="49"/>
         <v>7143.2</v>
       </c>
       <c r="E112" s="11">
-        <f>$G$96/E106</f>
+        <f t="shared" si="49"/>
         <v>2294.88</v>
       </c>
       <c r="F112" s="11">
-        <f>$G$96/F106</f>
+        <f t="shared" si="49"/>
         <v>1848.32</v>
       </c>
       <c r="G112" s="11">
-        <f>$G$96/G106</f>
+        <f t="shared" si="49"/>
         <v>79.999999999999986</v>
       </c>
       <c r="H112" s="11">
-        <f>$G$96/H106</f>
+        <f t="shared" si="49"/>
         <v>133.77199999999999</v>
       </c>
     </row>
@@ -8542,27 +10012,27 @@
         <v>int32</v>
       </c>
       <c r="C113" s="11">
-        <f>$G$96/C107</f>
+        <f t="shared" si="49"/>
         <v>8015.9999999999991</v>
       </c>
       <c r="D113" s="11">
-        <f>$G$96/D107</f>
+        <f t="shared" si="49"/>
         <v>647.28</v>
       </c>
       <c r="E113" s="11">
-        <f>$G$96/E107</f>
+        <f t="shared" si="49"/>
         <v>393.68</v>
       </c>
       <c r="F113" s="11">
-        <f>$G$96/F107</f>
+        <f t="shared" si="49"/>
         <v>129.59999999999997</v>
       </c>
       <c r="G113" s="11">
-        <f>$G$96/G107</f>
+        <f t="shared" si="49"/>
         <v>85.6</v>
       </c>
       <c r="H113" s="11">
-        <f>$G$96/H107</f>
+        <f t="shared" si="49"/>
         <v>70.152000000000001</v>
       </c>
     </row>
@@ -8572,27 +10042,27 @@
         <v>int16</v>
       </c>
       <c r="C114" s="11">
-        <f>$G$96/C108</f>
+        <f t="shared" si="49"/>
         <v>2464</v>
       </c>
       <c r="D114" s="11">
-        <f>$G$96/D108</f>
+        <f t="shared" si="49"/>
         <v>540.39999999999986</v>
       </c>
       <c r="E114" s="11">
-        <f>$G$96/E108</f>
+        <f t="shared" si="49"/>
         <v>393.68</v>
       </c>
       <c r="F114" s="11">
-        <f>$G$96/F108</f>
+        <f t="shared" si="49"/>
         <v>129.59999999999997</v>
       </c>
       <c r="G114" s="11">
-        <f>$G$96/G108</f>
+        <f t="shared" si="49"/>
         <v>85.6</v>
       </c>
       <c r="H114" s="11">
-        <f>$G$96/H108</f>
+        <f t="shared" si="49"/>
         <v>70.152000000000001</v>
       </c>
     </row>
@@ -8644,8 +10114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="S34" sqref="S34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8691,6 +10161,15 @@
       <c r="E9" t="s">
         <v>88</v>
       </c>
+      <c r="G9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I9" t="s">
+        <v>70</v>
+      </c>
       <c r="K9"/>
       <c r="L9"/>
     </row>
@@ -8707,6 +10186,18 @@
       <c r="E10" t="s">
         <v>63</v>
       </c>
+      <c r="G10" t="str">
+        <f>C10</f>
+        <v>float</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" ref="H10:I10" si="0">D10</f>
+        <v>int16</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>int32</v>
+      </c>
       <c r="K10"/>
       <c r="L10"/>
     </row>
@@ -8737,6 +10228,18 @@
       <c r="E13">
         <v>129</v>
       </c>
+      <c r="G13" s="11">
+        <f>1000000/C13</f>
+        <v>3215.4340836012861</v>
+      </c>
+      <c r="H13" s="11">
+        <f t="shared" ref="H13:I13" si="1">1000000/D13</f>
+        <v>24390.243902439026</v>
+      </c>
+      <c r="I13" s="11">
+        <f t="shared" si="1"/>
+        <v>7751.937984496124</v>
+      </c>
       <c r="K13"/>
       <c r="L13"/>
     </row>
@@ -8753,6 +10256,18 @@
       <c r="E14">
         <v>254</v>
       </c>
+      <c r="G14" s="11">
+        <f t="shared" ref="G14:G16" si="2">1000000/C14</f>
+        <v>1607.7170418006431</v>
+      </c>
+      <c r="H14" s="11">
+        <f t="shared" ref="H14:H16" si="3">1000000/D14</f>
+        <v>12658.227848101265</v>
+      </c>
+      <c r="I14" s="11">
+        <f t="shared" ref="I14:I16" si="4">1000000/E14</f>
+        <v>3937.0078740157483</v>
+      </c>
       <c r="K14"/>
       <c r="L14"/>
     </row>
@@ -8769,6 +10284,18 @@
       <c r="E15">
         <v>503</v>
       </c>
+      <c r="G15" s="11">
+        <f t="shared" si="2"/>
+        <v>787.40157480314963</v>
+      </c>
+      <c r="H15" s="11">
+        <f t="shared" si="3"/>
+        <v>6451.6129032258068</v>
+      </c>
+      <c r="I15" s="11">
+        <f t="shared" si="4"/>
+        <v>1988.0715705765408</v>
+      </c>
       <c r="K15"/>
       <c r="L15"/>
     </row>
@@ -8784,6 +10311,18 @@
       </c>
       <c r="E16">
         <v>1002</v>
+      </c>
+      <c r="G16" s="11">
+        <f t="shared" si="2"/>
+        <v>396.51070578905632</v>
+      </c>
+      <c r="H16" s="11">
+        <f t="shared" si="3"/>
+        <v>3246.7532467532469</v>
+      </c>
+      <c r="I16" s="11">
+        <f t="shared" si="4"/>
+        <v>998.00399201596804</v>
       </c>
       <c r="K16"/>
       <c r="L16"/>

</xml_diff>

<commit_message>
Benchmark: additional analyses in XLSs
</commit_message>
<xml_diff>
--- a/Arduino/Audio Processing Benchmarking/FIR Speed Results.xlsx
+++ b/Arduino/Audio Processing Benchmarking/FIR Speed Results.xlsx
@@ -16,7 +16,7 @@
     <sheet name="NXP K66" sheetId="9" r:id="rId7"/>
     <sheet name="Python" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" calcOnSave="0"/>
 </workbook>
 </file>
 
@@ -1007,11 +1007,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="142080640"/>
-        <c:axId val="142087296"/>
+        <c:axId val="191803776"/>
+        <c:axId val="191806080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="142080640"/>
+        <c:axId val="191803776"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -1036,20 +1036,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142087296"/>
+        <c:crossAx val="191806080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="142087296"/>
+        <c:axId val="191806080"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1075,14 +1074,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142080640"/>
+        <c:crossAx val="191803776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
@@ -1152,15 +1150,17 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1600"/>
-              <a:t>FIR Performance,</a:t>
+              <a:t>FIR Filtering Performance,</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1600" baseline="0"/>
               <a:t> </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="1600"/>
-              <a:t>Naïve C</a:t>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Naive FIR</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -1168,12 +1168,10 @@
               <a:defRPr sz="1600"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1100"/>
-              <a:t>(Smaller</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100" baseline="0"/>
-              <a:t> is Better)</a:t>
+              <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>(Bigger is Better)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1100"/>
           </a:p>
@@ -1184,264 +1182,191 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.21079662231946025"/>
+          <c:y val="0.21795166229221347"/>
+          <c:w val="0.64403785561582649"/>
+          <c:h val="0.60956364829396326"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison!$B$61</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>int16</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Comparison!$Y$58:$AB$58</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Arduino Uno</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Arduino M0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Teensy 3.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>FRDM-K66F</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison!$Y$61:$AB$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10160.010160015239</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21645.351229957632</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44253.636380814365</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>54433.105395181738</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Arduino Uno'!$C$10</c:f>
+              <c:f>Comparison!$B$60</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>float</c:v>
+                  <c:v>int32</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="triangle"/>
-            <c:size val="7"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
+            <c:strRef>
+              <c:f>Comparison!$Y$58:$AB$58</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Arduino Uno</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Arduino M0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Teensy 3.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>FRDM-K66F</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>'Arduino Uno'!$B$13:$B$16</c:f>
+              <c:f>Comparison!$Y$60:$AB$60</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>5639.9596744324917</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>19795.674375415139</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>64</c:v>
+                  <c:v>44253.636380814365</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>128</c:v>
+                  <c:v>54433.105395181738</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison!$B$59</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>float</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Comparison!$Y$58:$AB$58</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Arduino Uno</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Arduino M0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Teensy 3.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>FRDM-K66F</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Arduino Uno'!$C$13:$C$16</c:f>
+              <c:f>Comparison!$Y$59:$AB$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>311</c:v>
+                  <c:v>3549.4260376644552</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>622</c:v>
+                  <c:v>5986.5081443669142</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1270</c:v>
+                  <c:v>11768.778828946262</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2522</c:v>
+                  <c:v>56568.542494923808</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Arduino Uno'!$D$10</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>int16</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="7"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Arduino Uno'!$B$13:$B$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>128</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Arduino Uno'!$D$13:$D$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>79</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>155</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>308</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Arduino Uno'!$E$10</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>int32</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="7"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Arduino Uno'!$B$13:$B$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>128</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Arduino Uno'!$E$13:$E$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>129</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>254</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>503</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1451,42 +1376,21 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="143115008"/>
-        <c:axId val="143117312"/>
-      </c:lineChart>
+        <c:gapWidth val="150"/>
+        <c:axId val="199108864"/>
+        <c:axId val="199127040"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="143115008"/>
+        <c:axId val="199108864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>FIR Length (samples)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143117312"/>
+        <c:crossAx val="199127040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1494,9 +1398,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="143117312"/>
+        <c:axId val="199127040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="60000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1512,35 +1417,34 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Duration (microseconds)</a:t>
+                  <a:t>Max Sample Rate (Hz) For FIR with Resolution of 250 Hz</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.4282560706401765E-2"/>
+              <c:y val="0.16239610673665791"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143115008"/>
+        <c:crossAx val="199108864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="10000"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.85346158319805399"/>
-          <c:y val="0.40029335261880306"/>
-          <c:w val="0.13112415861312135"/>
-          <c:h val="0.2337048183371167"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1607,7 +1511,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1881,11 +1784,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="142906112"/>
-        <c:axId val="142908416"/>
+        <c:axId val="192669952"/>
+        <c:axId val="192672512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="142906112"/>
+        <c:axId val="192669952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1907,14 +1810,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142908416"/>
+        <c:crossAx val="192672512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1922,9 +1824,8 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142908416"/>
+        <c:axId val="192672512"/>
         <c:scaling>
-          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1946,14 +1847,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142906112"/>
+        <c:crossAx val="192669952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2009,7 +1909,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1600"/>
-              <a:t>FIR Filters per Second,</a:t>
+              <a:t>FIR Performance,</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1600" baseline="0"/>
@@ -2026,17 +1926,16 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1100"/>
-              <a:t>(Bigger </a:t>
+              <a:t>(Smaller</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1100" baseline="0"/>
-              <a:t>is Better)</a:t>
+              <a:t> is Better)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1100"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2109,21 +2008,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Arduino Uno'!$G$13:$G$16</c:f>
+              <c:f>'Arduino Uno'!$C$13:$C$16</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3215.4340836012861</c:v>
+                  <c:v>311</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1607.7170418006431</c:v>
+                  <c:v>622</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>787.40157480314963</c:v>
+                  <c:v>1270</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>396.51070578905632</c:v>
+                  <c:v>2522</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2135,7 +2034,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Arduino Uno'!$H$10</c:f>
+              <c:f>'Arduino Uno'!$D$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2194,21 +2093,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Arduino Uno'!$H$13:$H$16</c:f>
+              <c:f>'Arduino Uno'!$D$13:$D$16</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>24390.243902439026</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12658.227848101265</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6451.6129032258068</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3246.7532467532469</c:v>
+                  <c:v>308</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2220,7 +2119,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Arduino Uno'!$I$10</c:f>
+              <c:f>'Arduino Uno'!$E$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2279,21 +2178,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Arduino Uno'!$I$13:$I$16</c:f>
+              <c:f>'Arduino Uno'!$E$13:$E$16</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7751.937984496124</c:v>
+                  <c:v>129</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3937.0078740157483</c:v>
+                  <c:v>254</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1988.0715705765408</c:v>
+                  <c:v>503</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>998.00399201596804</c:v>
+                  <c:v>1002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2310,11 +2209,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="142947072"/>
-        <c:axId val="142949376"/>
+        <c:axId val="193345792"/>
+        <c:axId val="193381120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="142947072"/>
+        <c:axId val="193345792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2336,14 +2235,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142949376"/>
+        <c:crossAx val="193381120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2351,11 +2249,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142949376"/>
+        <c:axId val="193381120"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:max val="48000"/>
-          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2371,22 +2268,20 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>FIR Filters per Second</a:t>
+                  <a:t>Duration (microseconds)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142947072"/>
+        <c:crossAx val="193345792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="8000"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2440,6 +2335,434 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1600"/>
+              <a:t>FIR Filters per Second,</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600"/>
+              <a:t>Naïve C</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>(Bigger </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t>is Better)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Arduino Uno'!$C$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>float</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Arduino Uno'!$B$13:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Arduino Uno'!$G$13:$G$16</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3215.4340836012861</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1607.7170418006431</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>787.40157480314963</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>396.51070578905632</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Arduino Uno'!$H$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>int16</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Arduino Uno'!$B$13:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Arduino Uno'!$H$13:$H$16</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>24390.243902439026</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12658.227848101265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6451.6129032258068</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3246.7532467532469</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Arduino Uno'!$I$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>int32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Arduino Uno'!$B$13:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Arduino Uno'!$I$13:$I$16</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7751.937984496124</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3937.0078740157483</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1988.0715705765408</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>998.00399201596804</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="193894656"/>
+        <c:axId val="193905408"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="193894656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>FIR Length (samples)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="193905408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="193905408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="48000"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>FIR Filters per Second</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="193894656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="8000"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.85346158319805399"/>
+          <c:y val="0.40029335261880306"/>
+          <c:w val="0.13112415861312135"/>
+          <c:h val="0.2337048183371167"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600"/>
               <a:t>FIR Performance,</a:t>
             </a:r>
             <a:r>
@@ -2467,7 +2790,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2765,11 +3087,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="143001088"/>
-        <c:axId val="143011840"/>
+        <c:axId val="194145280"/>
+        <c:axId val="194147840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="143001088"/>
+        <c:axId val="194145280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2791,14 +3113,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143011840"/>
+        <c:crossAx val="194147840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2806,7 +3127,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="143011840"/>
+        <c:axId val="194147840"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2831,14 +3152,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143001088"/>
+        <c:crossAx val="194145280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2869,7 +3189,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3016,11 +3336,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="141850880"/>
-        <c:axId val="141877632"/>
+        <c:axId val="194457600"/>
+        <c:axId val="194459520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="141850880"/>
+        <c:axId val="194457600"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -3049,13 +3369,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="141877632"/>
+        <c:crossAx val="194459520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="141877632"/>
+        <c:axId val="194459520"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3085,7 +3405,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141850880"/>
+        <c:crossAx val="194457600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3106,7 +3426,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3253,11 +3573,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="141972224"/>
-        <c:axId val="141974144"/>
+        <c:axId val="194476288"/>
+        <c:axId val="194498944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="141972224"/>
+        <c:axId val="194476288"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -3286,13 +3606,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141974144"/>
+        <c:crossAx val="194498944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="141974144"/>
+        <c:axId val="194498944"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3322,7 +3642,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141972224"/>
+        <c:crossAx val="194476288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3610,11 +3930,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="142134272"/>
-        <c:axId val="142136064"/>
+        <c:axId val="191836928"/>
+        <c:axId val="191838464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="142134272"/>
+        <c:axId val="191836928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3623,7 +3943,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142136064"/>
+        <c:crossAx val="191838464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3631,7 +3951,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142136064"/>
+        <c:axId val="191838464"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3662,7 +3982,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142134272"/>
+        <c:crossAx val="191836928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3954,11 +4274,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="142686848"/>
-        <c:axId val="142688640"/>
+        <c:axId val="191861120"/>
+        <c:axId val="191862656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="142686848"/>
+        <c:axId val="191861120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3967,7 +4287,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142688640"/>
+        <c:crossAx val="191862656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3975,7 +4295,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142688640"/>
+        <c:axId val="191862656"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4006,7 +4326,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142686848"/>
+        <c:crossAx val="191861120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4298,11 +4618,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="142729216"/>
-        <c:axId val="142730752"/>
+        <c:axId val="191901696"/>
+        <c:axId val="191903232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="142729216"/>
+        <c:axId val="191901696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4311,7 +4631,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142730752"/>
+        <c:crossAx val="191903232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4319,7 +4639,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142730752"/>
+        <c:axId val="191903232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4356,7 +4676,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142729216"/>
+        <c:crossAx val="191901696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10000"/>
@@ -4658,11 +4978,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="142744960"/>
-        <c:axId val="142783616"/>
+        <c:axId val="191921536"/>
+        <c:axId val="191927424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="142744960"/>
+        <c:axId val="191921536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4671,7 +4991,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="142783616"/>
+        <c:crossAx val="191927424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4679,7 +4999,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142783616"/>
+        <c:axId val="191927424"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4722,7 +5042,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142744960"/>
+        <c:crossAx val="191921536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5023,11 +5343,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="142546816"/>
-        <c:axId val="142548352"/>
+        <c:axId val="192162816"/>
+        <c:axId val="192168704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="142546816"/>
+        <c:axId val="192162816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5036,7 +5356,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142548352"/>
+        <c:crossAx val="192168704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5044,7 +5364,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142548352"/>
+        <c:axId val="192168704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5081,7 +5401,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142546816"/>
+        <c:crossAx val="192162816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5389,11 +5709,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="142587008"/>
-        <c:axId val="142588544"/>
+        <c:axId val="192199296"/>
+        <c:axId val="192414080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="142587008"/>
+        <c:axId val="192199296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5402,7 +5722,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142588544"/>
+        <c:crossAx val="192414080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5410,7 +5730,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142588544"/>
+        <c:axId val="192414080"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5448,7 +5768,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142587008"/>
+        <c:crossAx val="192199296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5765,11 +6085,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="142623488"/>
-        <c:axId val="142625408"/>
+        <c:axId val="192448768"/>
+        <c:axId val="192467328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="142623488"/>
+        <c:axId val="192448768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5791,14 +6111,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142625408"/>
+        <c:crossAx val="192467328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5806,7 +6125,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142625408"/>
+        <c:axId val="192467328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5829,14 +6148,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142623488"/>
+        <c:crossAx val="192448768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6153,11 +6471,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="143069568"/>
-        <c:axId val="143071488"/>
+        <c:axId val="192555264"/>
+        <c:axId val="192557440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="143069568"/>
+        <c:axId val="192555264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6179,14 +6497,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143071488"/>
+        <c:crossAx val="192557440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6194,7 +6511,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="143071488"/>
+        <c:axId val="192557440"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -6218,14 +6535,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143069568"/>
+        <c:crossAx val="192555264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6537,6 +6853,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>476252</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>171452</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="15" name="Chart 14"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7323,10 +7671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X114"/>
+  <dimension ref="A1:AB114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="E52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB84" sqref="AB84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9173,7 +9521,7 @@
         <v>35.12373132626297</v>
       </c>
     </row>
-    <row r="57" spans="2:9" s="13" customFormat="1">
+    <row r="57" spans="2:28" s="13" customFormat="1">
       <c r="B57" s="13" t="s">
         <v>44</v>
       </c>
@@ -9184,7 +9532,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="2:9">
+    <row r="58" spans="2:28">
       <c r="C58" t="str">
         <f t="shared" ref="C58:H58" si="39">C$21</f>
         <v>Arduino Uno</v>
@@ -9209,8 +9557,24 @@
         <f t="shared" si="39"/>
         <v>Python, PC</v>
       </c>
-    </row>
-    <row r="59" spans="2:9">
+      <c r="Y58" t="str">
+        <f>C58</f>
+        <v>Arduino Uno</v>
+      </c>
+      <c r="Z58" t="str">
+        <f t="shared" ref="Z58" si="40">D58</f>
+        <v>Arduino M0</v>
+      </c>
+      <c r="AA58" t="str">
+        <f>F58</f>
+        <v>Teensy 3.2</v>
+      </c>
+      <c r="AB58" t="str">
+        <f>G58</f>
+        <v>FRDM-K66F</v>
+      </c>
+    </row>
+    <row r="59" spans="2:28">
       <c r="B59" t="str">
         <f>$A$24</f>
         <v>float</v>
@@ -9242,8 +9606,28 @@
       <c r="I59" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="60" spans="2:9">
+      <c r="X59" t="str">
+        <f>B59</f>
+        <v>float</v>
+      </c>
+      <c r="Y59">
+        <f t="shared" ref="Y59:Y61" si="41">C59</f>
+        <v>3549.4260376644552</v>
+      </c>
+      <c r="Z59">
+        <f t="shared" ref="Z59:Z61" si="42">D59</f>
+        <v>5986.5081443669142</v>
+      </c>
+      <c r="AA59">
+        <f t="shared" ref="AA59:AA61" si="43">F59</f>
+        <v>11768.778828946262</v>
+      </c>
+      <c r="AB59">
+        <f t="shared" ref="AB59:AB61" si="44">G59</f>
+        <v>56568.542494923808</v>
+      </c>
+    </row>
+    <row r="60" spans="2:28">
       <c r="B60" t="str">
         <f>$A$28</f>
         <v>int32</v>
@@ -9275,8 +9659,28 @@
       <c r="I60" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="61" spans="2:9">
+      <c r="X60" t="str">
+        <f t="shared" ref="X60:X61" si="45">B60</f>
+        <v>int32</v>
+      </c>
+      <c r="Y60">
+        <f t="shared" si="41"/>
+        <v>5639.9596744324917</v>
+      </c>
+      <c r="Z60">
+        <f t="shared" si="42"/>
+        <v>19795.674375415139</v>
+      </c>
+      <c r="AA60">
+        <f t="shared" si="43"/>
+        <v>44253.636380814365</v>
+      </c>
+      <c r="AB60">
+        <f t="shared" si="44"/>
+        <v>54433.105395181738</v>
+      </c>
+    </row>
+    <row r="61" spans="2:28">
       <c r="B61" t="str">
         <f>$A$32</f>
         <v>int16</v>
@@ -9307,6 +9711,26 @@
       </c>
       <c r="I61" t="s">
         <v>45</v>
+      </c>
+      <c r="X61" t="str">
+        <f t="shared" si="45"/>
+        <v>int16</v>
+      </c>
+      <c r="Y61">
+        <f t="shared" si="41"/>
+        <v>10160.010160015239</v>
+      </c>
+      <c r="Z61">
+        <f t="shared" si="42"/>
+        <v>21645.351229957632</v>
+      </c>
+      <c r="AA61">
+        <f t="shared" si="43"/>
+        <v>44253.636380814365</v>
+      </c>
+      <c r="AB61">
+        <f t="shared" si="44"/>
+        <v>54433.105395181738</v>
       </c>
     </row>
     <row r="79" spans="2:7" s="12" customFormat="1">
@@ -9352,7 +9776,7 @@
     </row>
     <row r="82" spans="1:8">
       <c r="B82" t="str">
-        <f t="shared" ref="B82:B94" si="40">B23</f>
+        <f t="shared" ref="B82:B94" si="46">B23</f>
         <v>N_FIR</v>
       </c>
       <c r="C82" t="s">
@@ -9377,108 +9801,108 @@
         <v>float</v>
       </c>
       <c r="B83">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>16</v>
       </c>
       <c r="C83" s="11">
-        <f t="shared" ref="C83:G94" si="41">1000000/C24</f>
+        <f t="shared" ref="C83:G94" si="47">1000000/C24</f>
         <v>3215.4340836012861</v>
       </c>
       <c r="D83" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>8708.52564660803</v>
       </c>
       <c r="E83" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>28019.052956010088</v>
       </c>
       <c r="F83" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>34199.726402188782</v>
       </c>
       <c r="G83" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>769230.76923076925</v>
       </c>
       <c r="H83" s="11"/>
     </row>
     <row r="84" spans="1:8">
       <c r="B84">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>32</v>
       </c>
       <c r="C84" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>1607.7170418006431</v>
       </c>
       <c r="D84" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>4415.5958846646354</v>
       </c>
       <c r="E84" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>13958.682300390843</v>
       </c>
       <c r="F84" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>17226.528854435834</v>
       </c>
       <c r="G84" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>370370.37037037034</v>
       </c>
       <c r="H84" s="11"/>
     </row>
     <row r="85" spans="1:8">
       <c r="B85">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>64</v>
       </c>
       <c r="C85" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>787.40157480314963</v>
       </c>
       <c r="D85" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>2239.8924851607126</v>
       </c>
       <c r="E85" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>6972.0421111343512</v>
       </c>
       <c r="F85" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>8656.5096952908589</v>
       </c>
       <c r="G85" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>200000</v>
       </c>
       <c r="H85" s="11"/>
     </row>
     <row r="86" spans="1:8">
       <c r="B86">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>128</v>
       </c>
       <c r="C86" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>396.51070578905632</v>
       </c>
       <c r="D86" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>1120.1469632815824</v>
       </c>
       <c r="E86" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>3485.1705991008257</v>
       </c>
       <c r="F86" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>4338.5830187860647</v>
       </c>
       <c r="G86" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>100000</v>
       </c>
       <c r="H86" s="11"/>
@@ -9489,108 +9913,108 @@
         <v>int32</v>
       </c>
       <c r="B87">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>16</v>
       </c>
       <c r="C87" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>7751.937984496124</v>
       </c>
       <c r="D87" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>92850.510677808736</v>
       </c>
       <c r="E87" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>154083.20493066256</v>
       </c>
       <c r="F87" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>462962.96296296292</v>
       </c>
       <c r="G87" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>714285.71428571432</v>
       </c>
       <c r="H87" s="11"/>
     </row>
     <row r="88" spans="1:8">
       <c r="B88">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>32</v>
       </c>
       <c r="C88" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>3937.0078740157483</v>
       </c>
       <c r="D88" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>48100.048100048101</v>
       </c>
       <c r="E88" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>79365.079365079364</v>
       </c>
       <c r="F88" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>240384.61538461538</v>
       </c>
       <c r="G88" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>357142.85714285716</v>
       </c>
       <c r="H88" s="11"/>
     </row>
     <row r="89" spans="1:8">
       <c r="B89">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>64</v>
       </c>
       <c r="C89" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>1988.0715705765408</v>
       </c>
       <c r="D89" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>24491.795248591723</v>
       </c>
       <c r="E89" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>40322.580645161288</v>
       </c>
       <c r="F89" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>122399.02080783354</v>
       </c>
       <c r="G89" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>185185.18518518517</v>
       </c>
       <c r="H89" s="11"/>
     </row>
     <row r="90" spans="1:8">
       <c r="B90">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>128</v>
       </c>
       <c r="C90" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>998.00399201596804</v>
       </c>
       <c r="D90" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>12359.411692003461</v>
       </c>
       <c r="E90" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>20321.072952651899</v>
       </c>
       <c r="F90" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>61728.395061728399</v>
       </c>
       <c r="G90" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>93457.943925233645</v>
       </c>
       <c r="H90" s="11"/>
@@ -9601,108 +10025,108 @@
         <v>int16</v>
       </c>
       <c r="B91">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>16</v>
       </c>
       <c r="C91" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>24390.243902439026</v>
       </c>
       <c r="D91" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>109769.48408342482</v>
       </c>
       <c r="E91" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>154083.20493066256</v>
       </c>
       <c r="F91" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>462962.96296296292</v>
       </c>
       <c r="G91" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>714285.71428571432</v>
       </c>
       <c r="H91" s="11"/>
     </row>
     <row r="92" spans="1:8">
       <c r="B92">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>32</v>
       </c>
       <c r="C92" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>12658.227848101265</v>
       </c>
       <c r="D92" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>57273.768613974797</v>
       </c>
       <c r="E92" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>79365.079365079364</v>
       </c>
       <c r="F92" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>240384.61538461538</v>
       </c>
       <c r="G92" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>357142.85714285716</v>
       </c>
       <c r="H92" s="11"/>
     </row>
     <row r="93" spans="1:8">
       <c r="B93">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>64</v>
       </c>
       <c r="C93" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>6451.6129032258068</v>
       </c>
       <c r="D93" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>29282.576866764277</v>
       </c>
       <c r="E93" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>40322.580645161288</v>
       </c>
       <c r="F93" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>122399.02080783354</v>
       </c>
       <c r="G93" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>185185.18518518517</v>
       </c>
       <c r="H93" s="11"/>
     </row>
     <row r="94" spans="1:8">
       <c r="B94">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>128</v>
       </c>
       <c r="C94" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>3246.7532467532469</v>
       </c>
       <c r="D94" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>14803.849000740192</v>
       </c>
       <c r="E94" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>20321.072952651899</v>
       </c>
       <c r="F94" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>61728.395061728399</v>
       </c>
       <c r="G94" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>93457.943925233645</v>
       </c>
       <c r="H94" s="11"/>
@@ -9725,27 +10149,27 @@
     </row>
     <row r="99" spans="2:8">
       <c r="C99" t="str">
-        <f t="shared" ref="C99:H99" si="42">C$21</f>
+        <f t="shared" ref="C99:H99" si="48">C$21</f>
         <v>Arduino Uno</v>
       </c>
       <c r="D99" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>Arduino M0</v>
       </c>
       <c r="E99" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>Arduino Due</v>
       </c>
       <c r="F99" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>Teensy 3.2</v>
       </c>
       <c r="G99" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>FRDM-K66F</v>
       </c>
       <c r="H99" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>Python, PC</v>
       </c>
     </row>
@@ -9759,7 +10183,7 @@
         <v>1.9843749999999998E-5</v>
       </c>
       <c r="D100">
-        <f t="shared" ref="D100" si="43">D26*0.000001/$B26</f>
+        <f t="shared" ref="D100" si="49">D26*0.000001/$B26</f>
         <v>6.9757812499999997E-6</v>
       </c>
       <c r="E100">
@@ -9789,7 +10213,7 @@
         <v>7.8281249999999988E-6</v>
       </c>
       <c r="D101">
-        <f t="shared" ref="D101" si="44">D31*0.000001/$B31</f>
+        <f t="shared" ref="D101" si="50">D31*0.000001/$B31</f>
         <v>6.3210937499999997E-7</v>
       </c>
       <c r="E101">
@@ -9819,7 +10243,7 @@
         <v>2.40625E-6</v>
       </c>
       <c r="D102">
-        <f t="shared" ref="D102" si="45">D35*0.000001/$B35</f>
+        <f t="shared" ref="D102" si="51">D35*0.000001/$B35</f>
         <v>5.2773437499999991E-7</v>
       </c>
       <c r="E102">
@@ -9846,27 +10270,27 @@
     </row>
     <row r="105" spans="2:8">
       <c r="C105" t="str">
-        <f t="shared" ref="C105:H105" si="46">C$21</f>
+        <f t="shared" ref="C105:H105" si="52">C$21</f>
         <v>Arduino Uno</v>
       </c>
       <c r="D105" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="52"/>
         <v>Arduino M0</v>
       </c>
       <c r="E105" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="52"/>
         <v>Arduino Due</v>
       </c>
       <c r="F105" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="52"/>
         <v>Teensy 3.2</v>
       </c>
       <c r="G105" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="52"/>
         <v>FRDM-K66F</v>
       </c>
       <c r="H105" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="52"/>
         <v>Python, PC</v>
       </c>
     </row>
@@ -9876,27 +10300,27 @@
         <v>float</v>
       </c>
       <c r="C106" s="10">
-        <f t="shared" ref="C106:H108" si="47">(1/$G$96)/C100</f>
+        <f t="shared" ref="C106:H108" si="53">(1/$G$96)/C100</f>
         <v>1.5748031496062995</v>
       </c>
       <c r="D106" s="10">
-        <f t="shared" si="47"/>
+        <f t="shared" si="53"/>
         <v>4.4797849703214245</v>
       </c>
       <c r="E106" s="10">
-        <f t="shared" si="47"/>
+        <f t="shared" si="53"/>
         <v>13.944084222268703</v>
       </c>
       <c r="F106" s="10">
-        <f t="shared" si="47"/>
+        <f t="shared" si="53"/>
         <v>17.313019390581719</v>
       </c>
       <c r="G106" s="10">
-        <f t="shared" si="47"/>
+        <f t="shared" si="53"/>
         <v>400.00000000000006</v>
       </c>
       <c r="H106" s="10">
-        <f t="shared" si="47"/>
+        <f t="shared" si="53"/>
         <v>239.21298926531713</v>
       </c>
     </row>
@@ -9906,27 +10330,27 @@
         <v>int32</v>
       </c>
       <c r="C107" s="10">
-        <f t="shared" si="47"/>
+        <f t="shared" si="53"/>
         <v>3.9920159680638729</v>
       </c>
       <c r="D107" s="10">
-        <f t="shared" si="47"/>
+        <f t="shared" si="53"/>
         <v>49.437646768013849</v>
       </c>
       <c r="E107" s="10">
-        <f t="shared" si="47"/>
+        <f t="shared" si="53"/>
         <v>81.284291810607598</v>
       </c>
       <c r="F107" s="10">
-        <f t="shared" si="47"/>
+        <f t="shared" si="53"/>
         <v>246.91358024691363</v>
       </c>
       <c r="G107" s="10">
-        <f t="shared" si="47"/>
+        <f t="shared" si="53"/>
         <v>373.8317757009346</v>
       </c>
       <c r="H107" s="10">
-        <f t="shared" si="47"/>
+        <f t="shared" si="53"/>
         <v>456.15235488653212</v>
       </c>
     </row>
@@ -9936,27 +10360,27 @@
         <v>int16</v>
       </c>
       <c r="C108" s="10">
-        <f t="shared" si="47"/>
+        <f t="shared" si="53"/>
         <v>12.987012987012987</v>
       </c>
       <c r="D108" s="10">
-        <f t="shared" si="47"/>
+        <f t="shared" si="53"/>
         <v>59.21539600296078</v>
       </c>
       <c r="E108" s="10">
-        <f t="shared" si="47"/>
+        <f t="shared" si="53"/>
         <v>81.284291810607598</v>
       </c>
       <c r="F108" s="10">
-        <f t="shared" si="47"/>
+        <f t="shared" si="53"/>
         <v>246.91358024691363</v>
       </c>
       <c r="G108" s="10">
-        <f t="shared" si="47"/>
+        <f t="shared" si="53"/>
         <v>373.8317757009346</v>
       </c>
       <c r="H108" s="10">
-        <f t="shared" si="47"/>
+        <f t="shared" si="53"/>
         <v>456.15235488653212</v>
       </c>
     </row>
@@ -9967,27 +10391,27 @@
     </row>
     <row r="111" spans="2:8">
       <c r="C111" t="str">
-        <f t="shared" ref="C111:H111" si="48">C$21</f>
+        <f t="shared" ref="C111:H111" si="54">C$21</f>
         <v>Arduino Uno</v>
       </c>
       <c r="D111" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>Arduino M0</v>
       </c>
       <c r="E111" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>Arduino Due</v>
       </c>
       <c r="F111" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>Teensy 3.2</v>
       </c>
       <c r="G111" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>FRDM-K66F</v>
       </c>
       <c r="H111" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>Python, PC</v>
       </c>
     </row>
@@ -9997,27 +10421,27 @@
         <v>float</v>
       </c>
       <c r="C112" s="11">
-        <f t="shared" ref="C112:H114" si="49">$G$96/C106</f>
+        <f t="shared" ref="C112:H114" si="55">$G$96/C106</f>
         <v>20319.999999999996</v>
       </c>
       <c r="D112" s="11">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>7143.2</v>
       </c>
       <c r="E112" s="11">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>2294.88</v>
       </c>
       <c r="F112" s="11">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>1848.32</v>
       </c>
       <c r="G112" s="11">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>79.999999999999986</v>
       </c>
       <c r="H112" s="11">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>133.77199999999999</v>
       </c>
     </row>
@@ -10027,27 +10451,27 @@
         <v>int32</v>
       </c>
       <c r="C113" s="11">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>8015.9999999999991</v>
       </c>
       <c r="D113" s="11">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>647.28</v>
       </c>
       <c r="E113" s="11">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>393.68</v>
       </c>
       <c r="F113" s="11">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>129.59999999999997</v>
       </c>
       <c r="G113" s="11">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>85.6</v>
       </c>
       <c r="H113" s="11">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>70.152000000000001</v>
       </c>
     </row>
@@ -10057,27 +10481,27 @@
         <v>int16</v>
       </c>
       <c r="C114" s="11">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>2464</v>
       </c>
       <c r="D114" s="11">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>540.39999999999986</v>
       </c>
       <c r="E114" s="11">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>393.68</v>
       </c>
       <c r="F114" s="11">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>129.59999999999997</v>
       </c>
       <c r="G114" s="11">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>85.6</v>
       </c>
       <c r="H114" s="11">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>70.152000000000001</v>
       </c>
     </row>

</xml_diff>